<commit_message>
Converted file from .xls to .xlsx format to fix error where testing files could not open it
</commit_message>
<xml_diff>
--- a/testing/test_files/test_genome_annotation.xlsx
+++ b/testing/test_files/test_genome_annotation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1985937\Documents\BI_Sum_2021\EC-Scrape\testing\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D53C59C-B875-40B1-9A96-61AC54CB0D65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{397A6AE0-0746-4F39-91C3-E5E23ABFF3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Genome Annotation" sheetId="1" r:id="rId1"/>
@@ -1556,7 +1556,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8">
     <font>
       <sz val="10"/>
@@ -2056,12 +2056,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane activePane="bottomRight" state="frozen"/>
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2748,30 +2748,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.2"/>
-    <hyperlink ref="B3" r:id="rId2" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.13"/>
-    <hyperlink ref="B4" r:id="rId3" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.14"/>
-    <hyperlink ref="B5" r:id="rId4" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.15"/>
-    <hyperlink ref="B6" r:id="rId5" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.296"/>
-    <hyperlink ref="B7" r:id="rId6" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.297"/>
-    <hyperlink ref="B8" r:id="rId7" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.602"/>
-    <hyperlink ref="B9" r:id="rId8" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.835"/>
-    <hyperlink ref="B10" r:id="rId9" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.851"/>
-    <hyperlink ref="B11" r:id="rId10" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.852"/>
-    <hyperlink ref="B12" r:id="rId11" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.853"/>
-    <hyperlink ref="B13" r:id="rId12" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.854"/>
-    <hyperlink ref="B14" r:id="rId13" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.855"/>
-    <hyperlink ref="B15" r:id="rId14" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.856"/>
-    <hyperlink ref="B16" r:id="rId15" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.857"/>
-    <hyperlink ref="B17" r:id="rId16" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.858"/>
-    <hyperlink ref="B18" r:id="rId17" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.859"/>
-    <hyperlink ref="B19" r:id="rId18" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.860"/>
-    <hyperlink ref="B20" r:id="rId19" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.1111"/>
-    <hyperlink ref="H9" r:id="rId20"/>
-    <hyperlink ref="H10" r:id="rId21"/>
-    <hyperlink ref="H2" r:id="rId22"/>
-    <hyperlink ref="H3" r:id="rId23"/>
-    <hyperlink ref="H8" r:id="rId24"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.13" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.14" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.15" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.296" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.297" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.602" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.835" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.851" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.852" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B12" r:id="rId11" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.853" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B13" r:id="rId12" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.854" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B14" r:id="rId13" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.855" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B15" r:id="rId14" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.856" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B16" r:id="rId15" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.857" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B17" r:id="rId16" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.858" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B18" r:id="rId17" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.859" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B19" r:id="rId18" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.860" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B20" r:id="rId19" display="http://rast.nmpdr.org//seedviewer.cgi?page=Annotation&amp;feature=fig|6666666.783512.peg.1111" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="H9" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="H10" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="H2" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="H3" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="H8" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
   </hyperlinks>
   <printOptions gridLines="1" gridLinesSet="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2781,7 +2781,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K246"/>
   <sheetViews>
     <sheetView topLeftCell="A144" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -5792,542 +5792,542 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B6" location="'Genome Annotation'!H93" display="Zinc ABC transporter, substrate-binding protein ZnuA"/>
-    <hyperlink ref="C6" r:id="rId1" tooltip="Go to alignment for MULTISPECIES: metal ABC transporter substrate-binding protein [Geobacillus] &gt;gb|ABO68109.1| High-affinity zinc uptake system protein ZnuA [Geobacillus thermodenitrificans NG80-2] &gt;gb|ARA98737.1| adhesin [Geobacillus thermodenitrificans"/>
-    <hyperlink ref="B7" location="'Genome Annotation'!H104" display="ABC transporter, permease protein (cluster 10, nitrate/sulfonate/bicarbonate)"/>
-    <hyperlink ref="C7" r:id="rId2" display=" _x0009_MULTISPECIES: ABC transporter permease [Geobacillus]"/>
-    <hyperlink ref="B8" location="'Genome Annotation'!H105" display="ABC transporter, ATP-binding protein (cluster 1, maltose/g3p/polyamine/iron); ABC transporter, ATP-binding protein (cluster 10, nitrate/sulfonate/bicarbonate)"/>
-    <hyperlink ref="C8" r:id="rId3" tooltip="Go to alignment for MULTISPECIES: ABC transporter ATP-binding protein [Geobacillus] &gt;gb|ABO68100.1| Putative transporter [Geobacillus thermodenitrificans NG80-2] &gt;gb|ARP43864.1| putative ABC transporter ATP-binding protein [Geobacillus thermodenitrificans"/>
-    <hyperlink ref="B9" location="'Genome Annotation'!H106" display="ABC transporter, ATP-binding protein (cluster 1, maltose/g3p/polyamine/iron); ABC transporter, ATP-binding protein (cluster 10, nitrate/sulfonate/bicarbonate)"/>
-    <hyperlink ref="C9" r:id="rId4" tooltip="Go to alignment for MULTISPECIES: ABC transporter ATP-binding protein [Geobacillus] &gt;gb|ABO68100.1| Putative transporter [Geobacillus thermodenitrificans NG80-2] &gt;gb|ARP43864.1| putative ABC transporter ATP-binding protein [Geobacillus thermodenitrificans"/>
-    <hyperlink ref="B10" location="'Genome Annotation'!H107" display="ABC transporter, ATP-binding protein (cluster 1, maltose/g3p/polyamine/iron); ABC transporter, ATP-binding protein (cluster 10, nitrate/sulfonate/bicarbonate)"/>
-    <hyperlink ref="C10" r:id="rId5" tooltip="Go to alignment for ABC transporter ATP-binding protein [Geobacillus thermodenitrificans] &gt;gb|ARA98745.1| spermidine/putrescine ABC transporter ATP-binding protein [Geobacillus thermodenitrificans]"/>
-    <hyperlink ref="B11" location="'Genome Annotation'!H108" display="ABC transporter, substrate-binding protein (cluster 10, nitrate/sulfonate/bicarbonate)"/>
-    <hyperlink ref="C11" r:id="rId6" tooltip="Go to alignment for MULTISPECIES: ABC transporter substrate-binding protein [Geobacillus] &gt;gb|NNU86489.1| ABC transporter substrate-binding protein [Geobacillus sp. MR] &gt;gb|PJW22406.1| hypothetical protein CV632_03555 [Geobacillus thermodenitrificans]"/>
-    <hyperlink ref="B12" location="'Genome Annotation'!H109" display="ABC transporter, substrate-binding protein (cluster 10, nitrate/sulfonate/bicarbonate)"/>
-    <hyperlink ref="C12" r:id="rId7" tooltip="Go to alignment for NMT1/THI5 like protein [Geobacillus sp. BCO2]"/>
-    <hyperlink ref="B13" location="'Genome Annotation'!H110" display="ABC transporter, substrate-binding protein (cluster 10, nitrate/sulfonate/bicarbonate)"/>
-    <hyperlink ref="C13" r:id="rId8" tooltip="Go to alignment for ABC transporter substrate-binding protein [Geobacillus thermodenitrificans] &gt;gb|EDY05297.1| ABC transporter substrate-binding protein [Geobacillus thermodenitrificans]"/>
-    <hyperlink ref="B14" location="'Genome Annotation'!H312" display="Molybdenum ABC transporter, substrate-binding protein ModA"/>
-    <hyperlink ref="C14" r:id="rId9" tooltip="Go to alignment for MULTISPECIES: molybdate ABC transporter substrate-binding protein [Geobacillus] &gt;gb|OQP11615.1| molybdate ABC transporter substrate-binding protein [Geobacillus sp. 47C-IIb] &gt;gb|PTR46061.1| molybdate ABC transporter substrate-binding p"/>
-    <hyperlink ref="B15" location="'Genome Annotation'!H338" display="Alkanesulfonate ABC transporter substrate-binding protein SsuA"/>
-    <hyperlink ref="B16" location="'Genome Annotation'!H339" display="Alkanesulfonate ABC transporter substrate-binding protein SsuA"/>
-    <hyperlink ref="B17" location="'ABC Transporters'!H340" display="Alkanesulfonate ABC transporter permease protein SsuC"/>
-    <hyperlink ref="B18" location="'ABC Transporters'!H341" display="Alkanesulfonate ABC transporter permease protein SsuC"/>
-    <hyperlink ref="B19" location="'ABC Transporters'!H342" display="Alkanesulfonate ABC transporter permease protein SsuC"/>
-    <hyperlink ref="B20" location="'ABC Transporters'!H343" display="Alkanesulfonate ABC transporter ATP-binding protein SsuB"/>
-    <hyperlink ref="B21" location="'ABC Transporters'!H344" display="Alkanesulfonate ABC transporter ATP-binding protein SsuB"/>
-    <hyperlink ref="B22" location="'ABC Transporters'!H345" display="Alkanesulfonate ABC transporter substrate-binding protein SsuA"/>
-    <hyperlink ref="C15" r:id="rId10" tooltip="Go to alignment for Putative sulfonate binding protein precursor [Geobacillus thermodenitrificans NG80-2]"/>
-    <hyperlink ref="B23" location="'Genome Annotation'!H619" display="Zinc ABC transporter, ATP-binding protein ZnuC"/>
-    <hyperlink ref="B24" location="'Genome Annotation'!H620" display="Zinc ABC transporter, permease protein ZnuB"/>
-    <hyperlink ref="B25" location="'Genome Annotation'!H632" display="Phosphate ABC transporter, substrate-binding protein PstS (TC 3.A.1.7.1)"/>
-    <hyperlink ref="B26" location="'Genome Annotation'!H633" display="Phosphate ABC transporter, permease protein PstC (TC 3.A.1.7.1)"/>
-    <hyperlink ref="B27" location="'ABC Transporters'!H634" display="Phosphate ABC transporter, permease protein PstA (TC 3.A.1.7.1)"/>
-    <hyperlink ref="B28" location="'Genome Annotation'!H635" display="Phosphate ABC transporter, permease protein PstA (TC 3.A.1.7.1)"/>
-    <hyperlink ref="B29" location="'Genome Annotation'!H636" display="Phosphate ABC transporter, ATP-binding protein PstB (TC 3.A.1.7.1)"/>
-    <hyperlink ref="B30" location="'Genome Annotation'!H886" display="Vitamin B12 ABC transporter, substrate-binding protein BtuF"/>
-    <hyperlink ref="B31" location="'Genome Annotation'!H887" display="Vitamin B12 ABC transporter, substrate-binding protein BtuF"/>
-    <hyperlink ref="B32" location="'Genome Annotation'!H888" display="Vitamin B12 ABC transporter, permease protein BtuC"/>
-    <hyperlink ref="B33" location="'Genome Annotation'!H889" display="Vitamin B12 ABC transporter, ATP-binding protein BtuD / Adenosylcobinamide amidohydrolase (EC 3.5.1.90)"/>
-    <hyperlink ref="B34" location="'Genome Annotation'!H1139" display="Oligopeptide ABC transporter, permease protein OppC (TC 3.A.1.5.1)"/>
-    <hyperlink ref="B35" location="'Genome Annotation'!H1140" display="Oligopeptide ABC transporter, permease protein OppB (TC 3.A.1.5.1)"/>
-    <hyperlink ref="B36" location="'Genome Annotation'!H1141" display="Oligopeptide ABC transporter, permease protein OppB (TC 3.A.1.5.1)"/>
-    <hyperlink ref="C34" r:id="rId11" tooltip="Go to alignment for ABC transporter permease subunit [Geobacillus thermodenitrificans] &gt;gb|EDY05593.1| binding-protein-dependent transport systems inner membrane component [Geobacillus thermodenitrificans]"/>
-    <hyperlink ref="B37" location="'Genome Annotation'!H1146" display="Hydroxymethylpyrimidine ABC transporter, ATPase component"/>
-    <hyperlink ref="B38" location="'Genome Annotation'!H1147" display="Hydroxymethylpyrimidine ABC transporter, ATPase component"/>
-    <hyperlink ref="B39" location="'Genome Annotation'!H1148" display="Hydroxymethylpyrimidine ABC transporter, transmembrane component"/>
-    <hyperlink ref="B40" location="'Genome Annotation'!H1149" display="Hydroxymethylpyrimidine ABC transporter, substrate-binding component"/>
-    <hyperlink ref="B41" location="'Genome Annotation'!H1171" display="Maltodextrin ABC transporter, substrate-binding protein MdxE"/>
-    <hyperlink ref="B42" location="'Genome Annotation'!H1172" display="Maltodextrin ABC transporter, permease protein MdxF"/>
-    <hyperlink ref="B43" location="'Genome Annotation'!H1173" display="Maltodextrin ABC transporter, permease protein MdxG"/>
-    <hyperlink ref="B44" location="'Genome Annotation'!H1254" display="ABC transporter, permease protein"/>
-    <hyperlink ref="B45" location="'Genome Annotation'!H1255" display="ABC transporter, permease protein"/>
-    <hyperlink ref="B46" location="'Genome Annotation'!H1256" display="Efflux ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="B47" location="'Genome Annotation'!H1297" display="ABC transporter, substrate-binding protein (cluster 15, trp?)"/>
-    <hyperlink ref="B48" location="'Genome Annotation'!H1298" display="Predicted ABC transporter for tryptophane, permease protein TrpY"/>
-    <hyperlink ref="B49" location="'Genome Annotation'!H1299" display="ABC transporter, ATP-binding protein (cluster 15, trp?)"/>
-    <hyperlink ref="B50" location="'Genome Annotation'!H1310" display="Glycerol-3-phosphate ABC transporter, ATP-binding protein UgpC (TC 3.A.1.1.3)"/>
-    <hyperlink ref="B51" location="'Genome Annotation'!H1311" display="Glycerol-3-phosphate ABC transporter, ATP-binding protein UgpC (TC 3.A.1.1.3)"/>
-    <hyperlink ref="B52" location="'Genome Annotation'!H1312" display="Glycerol-3-phosphate ABC transporter, ATP-binding protein UgpC (TC 3.A.1.1.3)"/>
-    <hyperlink ref="B53" location="'Genome Annotation'!H1313" display="Glycerol-3-phosphate ABC transporter, permease protein UgpA (TC 3.A.1.1.3)"/>
-    <hyperlink ref="B54" location="'Genome Annotation'!H1314" display="Glycerol-3-phosphate ABC transporter, permease protein UgpE (TC 3.A.1.1.3)"/>
-    <hyperlink ref="B55" location="'Genome Annotation'!H1315" display="Glycerol-3-phosphate ABC transporter, substrate-binding protein UgpB"/>
-    <hyperlink ref="B56" location="'Genome Annotation'!H1316" display="Glycerol-3-phosphate ABC transporter, substrate-binding protein UgpB"/>
-    <hyperlink ref="B57" location="'Genome Annotation'!H1435" display="Urea ABC transporter, substrate-binding protein UrtA"/>
-    <hyperlink ref="B58" location="'Genome Annotation'!H1436" display="Urea ABC transporter, substrate-binding protein UrtA"/>
-    <hyperlink ref="B59" location="'Genome Annotation'!H1437" display="Urea ABC transporter, permease protein UrtB"/>
-    <hyperlink ref="B60" location="'Genome Annotation'!H1438" display="Urea ABC transporter, permease protein UrtB"/>
-    <hyperlink ref="B61" location="'Genome Annotation'!H1439" display="Urea ABC transporter, permease protein UrtC"/>
-    <hyperlink ref="B62" location="'Genome Annotation'!H1440" display="Urea ABC transporter, ATPase protein UrtD"/>
-    <hyperlink ref="B63" location="'Genome Annotation'!H1441" display="Urea ABC transporter, ATPase protein UrtD"/>
-    <hyperlink ref="B64" location="'Genome Annotation'!H1442" display="Urea ABC transporter, ATPase protein UrtE"/>
-    <hyperlink ref="B65" location="'Genome Annotation'!H1473" display="Maltose/maltodextrin ABC transporter, substrate binding periplasmic protein MalE"/>
-    <hyperlink ref="B66" location="'Genome Annotation'!H1477" display="Maltose/maltodextrin ABC transporter, substrate binding periplasmic protein MalE"/>
-    <hyperlink ref="B67" location="'Genome Annotation'!H1479" display="putative sugar ABC transporter, permease protein"/>
-    <hyperlink ref="C67" r:id="rId12" tooltip="Go to alignment for MULTISPECIES: carbohydrate ABC transporter permease [unclassified Geobacillus] &gt;gb|QNU31522.1| carbohydrate ABC transporter permease [Geobacillus sp. 47C-IIb] &gt;gb|RXS91429.1| carbohydrate ABC transporter permease [Geobacillus sp. PK12]"/>
-    <hyperlink ref="B68" location="'Genome Annotation'!H1495" display="ABC transporter, substrate-binding protein (cluster 2, ribose/xylose/arabinose/galactose)"/>
-    <hyperlink ref="B69" location="'Genome Annotation'!H1499" display="L-arabinose ABC transporter, substrate-binding protein AraF"/>
-    <hyperlink ref="B70" location="'Genome Annotation'!H1500" display="L-arabinose ABC transporter, ATP-binding protein AraG"/>
-    <hyperlink ref="B71" location="'Genome Annotation'!H1501" display="L-arabinose ABC transporter, permease protein AraH"/>
-    <hyperlink ref="B72" location="'Genome Annotation'!H1502" display="L-arabinose ABC transporter, permease protein AraH"/>
-    <hyperlink ref="B73" location="'Genome Annotation'!H1509" display="Alpha-arabinosides ABC transport system, substrate-binding protein AraN"/>
-    <hyperlink ref="B74" location="'Genome Annotation'!H1510" display="Alpha-arabinosides ABC transport system, permease protein AraP"/>
-    <hyperlink ref="B75" location="'Genome Annotation'!H1511" display="Alpha-arabinosides ABC transport system, permease protein AraQ"/>
-    <hyperlink ref="B76" location="'Genome Annotation'!H1525" display="Xylose ABC transporter, substrate-binding component"/>
-    <hyperlink ref="B77" location="'Genome Annotation'!H1526" display="ABC transporter, permease protein 1 (cluster 1, maltose/g3p/polyamine/iron)"/>
-    <hyperlink ref="B78" location="'Genome Annotation'!H1527" display="ABC transporter, permease protein 1 (cluster 1, maltose/g3p/polyamine/iron)"/>
-    <hyperlink ref="B79" location="'Genome Annotation'!H1528" display="Xylose ABC transporter, ATP-binding component"/>
-    <hyperlink ref="B80" location="'Genome Annotation'!H1534" display="ABC transporter, substrate-binding protein (cluster 1, maltose/g3p/polyamine/iron)"/>
-    <hyperlink ref="B81" location="'Genome Annotation'!H1535" display="ABC transporter, permease protein 1 (cluster 1, maltose/g3p/polyamine/iron)"/>
-    <hyperlink ref="B82" location="'Genome Annotation'!H1536" display="ABC transporter, permease protein 2 (cluster 1, maltose/g3p/polyamine/iron)"/>
-    <hyperlink ref="B83" location="'Genome Annotation'!H1886" display="ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="B84" location="'Genome Annotation'!H1900" display="ABC transporter, substrate-binding protein (cluster 4, leucine/isoleucine/valine/benzoate)"/>
-    <hyperlink ref="B85" location="'Genome Annotation'!H1901" display="ABC transporter, substrate-binding protein (cluster 4, leucine/isoleucine/valine/benzoate)"/>
-    <hyperlink ref="B86" location="'Genome Annotation'!H1902" display="ABC transporter, ATP-binding protein 1 (cluster 4, leucine/isoleucine/valine/benzoate)"/>
-    <hyperlink ref="B87" location="'Genome Annotation'!H1903" display="ABC transporter, permease protein 2 (cluster 4, leucine/isoleucine/valine/benzoate)"/>
-    <hyperlink ref="B88" location="'Genome Annotation'!H1904" display="ABC transporter, permease protein 2 (cluster 4, leucine/isoleucine/valine/benzoate)"/>
-    <hyperlink ref="B89" location="'Genome Annotation'!H1905" display="ABC transporter, permease protein 1 (cluster 4, leucine/isoleucine/valine/benzoate)"/>
-    <hyperlink ref="B90" location="'Genome Annotation'!H1906" display="ABC transporter, permease protein 1 (cluster 4, leucine/isoleucine/valine/benzoate)"/>
-    <hyperlink ref="B93" location="'Genome Annotation'!H1930" display="Efflux ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="B94" location="'Genome Annotation'!H1953" display="Efflux ABC transporter, permease/ATP-binding protein YfiC"/>
-    <hyperlink ref="B95" location="'Genome Annotation'!H1954" display="Efflux ABC transporter, permease/ATP-binding protein YfiB"/>
-    <hyperlink ref="B96" location="'Genome Annotation'!H1965" display="Efflux ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="B97" location="'Genome Annotation'!H2103" display="Efflux ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="B91" location="'Genome Annotation'!H1928" display="ABC transporter permease YhcI"/>
-    <hyperlink ref="B92" location="'Genome Annotation'!H1929" display="ABC transporter, permease protein"/>
-    <hyperlink ref="B98" location="'Genome Annotation'!H2104" display="ABC transporter, permease protein"/>
-    <hyperlink ref="B99" location="'Genome Annotation'!H2139" display="Methionine ABC transporter ATP-binding protein"/>
-    <hyperlink ref="B100" location="'Genome Annotation'!H2140" display="Methionine ABC transporter ATP-binding protein"/>
-    <hyperlink ref="B101" location="'Genome Annotation'!H2141" display="Methionine ABC transporter permease protein"/>
-    <hyperlink ref="B102" location="'Genome Annotation'!H2142" display="Methionine ABC transporter substrate-binding protein"/>
-    <hyperlink ref="B103" location="'Genome Annotation'!H2157" display="Efflux ABC transporter, permease protein"/>
-    <hyperlink ref="B104" location="'Genome Annotation'!H2158" display="Efflux ABC transporter, permease protein"/>
-    <hyperlink ref="B105" location="'Genome Annotation'!H2159" display="Efflux ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="B106:B107" location="'Genome Annotation'!H2178" display="ABC-type Fe3+-siderophore transport system, ATPase component"/>
-    <hyperlink ref="B108:B110" location="'Genome Annotation'!H2178" display="ABC-type Fe3+-siderophore transport system, permease 2 component"/>
-    <hyperlink ref="B107" location="'Genome Annotation'!H2179" display="ABC-type Fe3+-siderophore transport system, permease 2 component"/>
-    <hyperlink ref="B108" location="'Genome Annotation'!H2180" display="ABC-type Fe3+-siderophore transport system, permease 2 component"/>
-    <hyperlink ref="B109" location="'Genome Annotation'!H2181" display="ABC-type Fe3+-siderophore transport system, permease component"/>
-    <hyperlink ref="B110" location="'Genome Annotation'!H2182" display="ABC-type Fe3+-siderophore transport system, periplasmic iron-binding component"/>
-    <hyperlink ref="B111:B114" location="'ABC Transporters'!H2259" display="Uncharacterized iron compound ABC uptake transporter, substrate-binding protein"/>
-    <hyperlink ref="B112" location="'Genome Annotation'!H2260" display="Uncharacterized iron compound ABC uptake transporter, ATP-binding protein"/>
-    <hyperlink ref="B113" location="'Genome Annotation'!H2261" display="Uncharacterized iron compound ABC uptake transporter, permease protein"/>
-    <hyperlink ref="B114" location="'Genome Annotation'!H2262" display="Uncharacterized iron compound ABC uptake transporter, permease protein"/>
-    <hyperlink ref="B111" location="'Genome Annotation'!H2259" display="Uncharacterized iron compound ABC uptake transporter, substrate-binding protein"/>
-    <hyperlink ref="B115:B120" location="'Genome Annotation'!H2414" display="Efflux ABC transporter, permease/ATP-binding protein MdlB"/>
-    <hyperlink ref="B116" location="'Genome Annotation'!H2415" display="Efflux ABC transporter, permease/ATP-binding protein MdlB"/>
-    <hyperlink ref="B117" location="'Genome Annotation'!H2416" display="Efflux ABC transporter, permease/ATP-binding protein MdlB"/>
-    <hyperlink ref="B118" location="'Genome Annotation'!H2417" display="Efflux ABC transporter, permease/ATP-binding protein MdlA"/>
-    <hyperlink ref="B119" location="'Genome Annotation'!H2418" display="Efflux ABC transporter, permease/ATP-binding protein MdlA"/>
-    <hyperlink ref="B120" location="'Genome Annotation'!H2419" display="Efflux ABC transporter, permease/ATP-binding protein MdlA"/>
-    <hyperlink ref="B121" location="'Genome Annotation'!H2484" display="Transcriptional regulator in cluster with unspecified monosaccharide ABC transport system"/>
-    <hyperlink ref="B122:B125" location="'Genome Annotation'!H2494" display="Purine nucleoside ABC transporter, permease protein 2"/>
-    <hyperlink ref="B123" location="'Genome Annotation'!H2495" display="Purine nucleoside ABC transporter, permease protein 1"/>
-    <hyperlink ref="B124" location="'Genome Annotation'!H2496" display="Purine nucleoside ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="B125" location="'Genome Annotation'!H2498" display="Purine nucleoside ABC transporter, substrate-binding protein"/>
-    <hyperlink ref="B126" location="'Genome Annotation'!H2677" display="ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="B127:B128" location="'Genome Annotation'!H2931" display="Efflux ABC transporter, permease protein"/>
-    <hyperlink ref="B128" location="'Genome Annotation'!H2932" display="Efflux ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="B129:B132" location="'Genome Annotation'!H2957" display="5-methylthioribose ABC transporter, substrate-binding protein"/>
-    <hyperlink ref="B130" location="'Genome Annotation'!H2958" display="5-methylthioribose ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="B131" location="'Genome Annotation'!H2959" display="5-methylthioribose ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="B132" location="'Genome Annotation'!H2960" display="5-methylthioribose ABC transporter, permease protein"/>
-    <hyperlink ref="B133:B136" location="'Genome Annotation'!H2970" display="N-acetyl-D-glucosamine ABC transporter, permease protein 2"/>
-    <hyperlink ref="B134" location="'Genome Annotation'!H2971" display="N-acetyl-D-glucosamine ABC transporter, permease protein 1"/>
-    <hyperlink ref="B135" location="'Genome Annotation'!H2972" display="ABC transporter, substrate-binding protein (cluster 1, maltose/g3p/polyamine/iron)"/>
-    <hyperlink ref="B136" location="'Genome Annotation'!H2973" display="ABC transporter, substrate-binding protein (cluster 1, maltose/g3p/polyamine/iron)"/>
-    <hyperlink ref="B137:B140" location="'Genome Annotation'!H3016" display="Efflux ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="B138" location="'Genome Annotation'!H3017" display="Efflux ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="B139" location="'Genome Annotation'!H3018" display="Efflux ABC transporter, permease protein"/>
-    <hyperlink ref="B140" location="'Genome Annotation'!H3019" display="Efflux ABC transporter, permease protein"/>
-    <hyperlink ref="B141:B146" location="'Genome Annotation'!H3137" display="Oligopeptide ABC transporter, ATP-binding protein OppF (TC 3.A.1.5.1)"/>
-    <hyperlink ref="B142" location="'Genome Annotation'!H3138" display="Oligopeptide ABC transporter, ATP-binding protein OppD (TC 3.A.1.5.1)"/>
-    <hyperlink ref="B143" location="'Genome Annotation'!H3139" display="Oligopeptide ABC transporter, ATP-binding protein OppD (TC 3.A.1.5.1)"/>
-    <hyperlink ref="B144" location="'Genome Annotation'!H3140" display="Oligopeptide ABC transporter, permease protein OppC (TC 3.A.1.5.1)"/>
-    <hyperlink ref="B145" location="'Genome Annotation'!H3141" display="Oligopeptide ABC transporter, permease protein OppB (TC 3.A.1.5.1)"/>
-    <hyperlink ref="B146" location="'Genome Annotation'!H3142" display="ABC transporter, substrate-binding protein (cluster 5, nickel/peptides/opines)"/>
-    <hyperlink ref="B147" location="'Genome Annotation'!H3181" display="Molybdenum ABC transporter permease protein ModB"/>
-    <hyperlink ref="B148" location="'Genome Annotation'!H3229" display="Spermidine/putrescine import ABC transporter substrate-binding protein PotD (TC 3.A.1.11.1)"/>
-    <hyperlink ref="B149:B152" location="'Genome Annotation'!H3230" display="Spermidine/putrescine import ABC transporter permease protein PotC (TC 3.A.1.11.1)"/>
-    <hyperlink ref="B150" location="'Genome Annotation'!H3231" display="Spermidine/putrescine import ABC transporter permease protein PotB (TC 3.A.1.11.1)"/>
-    <hyperlink ref="B151" location="'Genome Annotation'!H3232" display="Spermidine/putrescine import ABC transporter ATP-binding protein PotA (TC 3.A.1.11.1)"/>
-    <hyperlink ref="B152" location="'Genome Annotation'!H3233" display="Spermidine/putrescine import ABC transporter ATP-binding protein PotA (TC 3.A.1.11.1)"/>
-    <hyperlink ref="B153:B155" location="'Genome Annotation'!H3249" display="Maltodextrin ABC transporter, permease protein MdxG"/>
-    <hyperlink ref="B154" location="'Genome Annotation'!H3250" display="Maltodextrin ABC transporter, permease protein MdxF"/>
-    <hyperlink ref="B155" location="'Genome Annotation'!H3251" display="Maltodextrin ABC transporter, substrate-binding protein MdxE"/>
-    <hyperlink ref="B156:B158" location="'Genome Annotation'!H3297" display="ABC transporter, ATP-binding protein (cluster 15, trp?)"/>
-    <hyperlink ref="B157" location="'Genome Annotation'!H3298" display="ABC transporter, permease protein (cluster 15, trp?)"/>
-    <hyperlink ref="B158" location="'Genome Annotation'!H3299" display="ABC transporter, substrate-binding protein (cluster 15, trp?)"/>
-    <hyperlink ref="B159:B160" location="'Genome Annotation'!H3311" display="ABC transporter, permease protein EscB"/>
-    <hyperlink ref="B160" location="'Genome Annotation'!H3312" display="ABC transporter, ATP-binding protein EcsA"/>
-    <hyperlink ref="B161:B162" location="'Genome Annotation'!H3329" display="ABC-type Na+ efflux pump, permease component"/>
-    <hyperlink ref="B162" location="'Genome Annotation'!H3330" display="Efflux ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="B163" location="'Genome Annotation'!H3344" display="Maltodextrin ABC transporter, ATP-binding protein MsmX"/>
-    <hyperlink ref="B164:B166" location="'Genome Annotation'!H3452" display="Efflux ABC transporter, permease protein"/>
-    <hyperlink ref="B165" location="'Genome Annotation'!H3453" display="Efflux ABC transporter, permease protein"/>
-    <hyperlink ref="B166" location="'Genome Annotation'!H3454" display="Efflux ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="B167:B174" location="'Genome Annotation'!H3480" display="Dipeptide ABC transporter, permease protein DppC (TC 3.A.1.5.2)"/>
-    <hyperlink ref="B168" location="'Genome Annotation'!H3481" display="Dipeptide ABC transporter, permease protein DppC (TC 3.A.1.5.2)"/>
-    <hyperlink ref="B169" location="'Genome Annotation'!H3482" display="Dipeptide ABC transporter, permease protein DppB (TC 3.A.1.5.2)"/>
-    <hyperlink ref="B170" location="'Genome Annotation'!H3483" display="Dipeptide ABC transporter, substrate-binding protein DppA (TC 3.A.1.5.2)"/>
-    <hyperlink ref="B171" location="'Genome Annotation'!H3484" display="Oligopeptide ABC transporter, ATP-binding protein OppF (TC 3.A.1.5.1)"/>
-    <hyperlink ref="B172" location="'Genome Annotation'!H3485" display="Oligopeptide ABC transporter, ATP-binding protein OppD (TC 3.A.1.5.1)"/>
-    <hyperlink ref="B173" location="'Genome Annotation'!H3486" display="Efflux ABC transporter, permease/ATP-binding protein YgaD"/>
-    <hyperlink ref="B174" location="'Genome Annotation'!H3487" display="Efflux ABC transporter, permease/ATP-binding protein YgaD"/>
-    <hyperlink ref="B175:B178" location="'Genome Annotation'!H3716" display="ABC transporter-coupled two-component system, ATP-binding protein"/>
-    <hyperlink ref="B176" location="'Genome Annotation'!H3717" display="ABC transporter-coupled two-component system, fused permease protein"/>
-    <hyperlink ref="B177" location="'Genome Annotation'!H3718" display="ABC transporter-coupled two-component system, LuxR family response regulator"/>
-    <hyperlink ref="B178" location="'Genome Annotation'!H3719" display="ABC transporter-coupled two-component system, signal transduction histidine kinase"/>
-    <hyperlink ref="B179" location="'Genome Annotation'!H3807" display="ABC transporter-like sensor and permease protein YxdM"/>
-    <hyperlink ref="B180" location="'Genome Annotation'!H3808" display="ABC transporter-like sensor ATP-binding protein YxdL"/>
-    <hyperlink ref="B181:B185" location="'Genome Annotation'!H3852" display="ABC transporter, substrate-binding protein (cluster 13, osmolytes)"/>
-    <hyperlink ref="B182" location="'Genome Annotation'!H3853" display="ABC transporter, substrate-binding protein (cluster 13, osmolytes)"/>
-    <hyperlink ref="B183" location="'Genome Annotation'!H3854" display="ABC transporter, ATP-binding protein (cluster 13, osmolytes)"/>
-    <hyperlink ref="B184" location="'Genome Annotation'!H3855" display="ABC transporter, permease protein (cluster 13, osmolytes)"/>
-    <hyperlink ref="B185" location="'Genome Annotation'!H3856" display="putative ABC transporter, ATP-binding protein MutF"/>
-    <hyperlink ref="B186:B187" location="'Genome Annotation'!H3857" display="Lantibiotic ABC transporter"/>
-    <hyperlink ref="B187" location="'Genome Annotation'!H3858" display="Lantibiotic ABC transporter"/>
-    <hyperlink ref="B188" location="'Genome Annotation'!H3950" display="Bis-ABC ATPase YheS"/>
-    <hyperlink ref="B189:B191" location="'Genome Annotation'!H4048" display="Oligopeptide ABC transporter, permease protein OppC (TC 3.A.1.5.1)"/>
-    <hyperlink ref="B190" location="'Genome Annotation'!H4049" display="Oligopeptide ABC transporter, permease protein OppB (TC 3.A.1.5.1)"/>
-    <hyperlink ref="B191" location="'Genome Annotation'!H4050" display="Oligopeptide ABC transporter, permease protein OppB (TC 3.A.1.5.1)"/>
-    <hyperlink ref="B192" location="'Genome Annotation'!H4057" display="ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="B193:B195" location="'Genome Annotation'!H4372" display="Efflux ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="B194" location="'Genome Annotation'!H4373" display="Export ABC transporter permease protein BA1794"/>
-    <hyperlink ref="B195" location="'Genome Annotation'!H4374" display="Export ABC transporter permease protein BA1795"/>
-    <hyperlink ref="B196:B199" location="'Genome Annotation'!H4403" display="ABC transporter, ATP-binding protein (cluster 3, basic aa/glutamine/opines)"/>
-    <hyperlink ref="B197" location="'Genome Annotation'!H4404" display="Glutamine ABC transporter, permease protein GlnP"/>
-    <hyperlink ref="B198" location="'Genome Annotation'!H4405" display="Glutamine ABC transporter, substrate-binding protein GlnH"/>
-    <hyperlink ref="B199" location="'Genome Annotation'!H4406" display="Glutamine ABC transporter, substrate-binding protein GlnH"/>
-    <hyperlink ref="B200:B201" location="'Genome Annotation'!H4552" display="Oligopeptide ABC transporter, ATP-binding protein OppD (TC 3.A.1.5.1)"/>
-    <hyperlink ref="B201" location="'Genome Annotation'!H4553" display="Oligopeptide ABC transporter, ATP-binding protein OppF (TC 3.A.1.5.1)"/>
-    <hyperlink ref="B202:B204" location="'Genome Annotation'!H4597" display="ABC transporter, substrate-binding protein (cluster 1, maltose/g3p/polyamine/iron)"/>
-    <hyperlink ref="B203" location="'Genome Annotation'!H4598" display="ABC transporter, substrate-binding protein (cluster 1, maltose/g3p/polyamine/iron)"/>
-    <hyperlink ref="B204" location="'Genome Annotation'!H4599" display="ABC transporter, permease protein 1 (cluster 1, maltose/g3p/polyamine/iron)"/>
-    <hyperlink ref="B205:B208" location="'Genome Annotation'!H4620" display="ABC transporter, substrate-binding protein (cluster 1, maltose/g3p/polyamine/iron)"/>
-    <hyperlink ref="B206" location="'Genome Annotation'!H4621" display="Spermidine/putrescine import ABC transporter ATP-binding protein PotA (TC 3.A.1.11.1)"/>
-    <hyperlink ref="B207" location="'Genome Annotation'!H4622" display="Spermidine/putrescine import ABC transporter permease protein PotB (TC 3.A.1.11.1)"/>
-    <hyperlink ref="B208" location="'Genome Annotation'!H4623" display="Spermidine/putrescine import ABC transporter permease protein PotC (TC 3.A.1.11.1)"/>
-    <hyperlink ref="B209:B211" location="'Genome Annotation'!H4658" display="Multiple sugar ABC transporter, substrate-binding protein MsmE"/>
-    <hyperlink ref="B210" location="'Genome Annotation'!H4659" display="Multiple sugar ABC transporter, permease protein MsmF"/>
-    <hyperlink ref="B211" location="'Genome Annotation'!H4660" display="Sugar ABC transporter, permease protein precursor"/>
-    <hyperlink ref="B212:B216" location="'Genome Annotation'!H4719" display="Ribose ABC transporter, ATP-binding protein RbsA (TC 3.A.1.2.1)"/>
-    <hyperlink ref="B213" location="'Genome Annotation'!H4720" display="Ribose ABC transporter, ATP-binding protein RbsA (TC 3.A.1.2.1)"/>
-    <hyperlink ref="B214" location="'Genome Annotation'!H4721" display="Ribose ABC transporter, permease protein RbsC (TC 3.A.1.2.1)"/>
-    <hyperlink ref="B215" location="'Genome Annotation'!H4722" display="Ribose ABC transporter, substrate-binding protein RbsB (TC 3.A.1.2.1)"/>
-    <hyperlink ref="B216" location="'Genome Annotation'!H4723" display="Ribose ABC transporter, substrate-binding protein RbsB (TC 3.A.1.2.1)"/>
-    <hyperlink ref="B217" location="'Genome Annotation'!H4763" display="Xylose ABC transporter, substrate-binding component"/>
-    <hyperlink ref="B218:B220" location="'Genome Annotation'!H4766" display="Predicted beta-glucoside-regulated ABC transport system, sugar binding component, COG1653"/>
-    <hyperlink ref="B219" location="'Genome Annotation'!H4767" display="Predicted beta-glucoside-regulated ABC transport system, permease component 1, COG1175"/>
-    <hyperlink ref="B220" location="'Genome Annotation'!H4768" display="Predicted beta-glucoside-regulated ABC transport system, permease component 2, COG0395"/>
-    <hyperlink ref="B221" location="'Genome Annotation'!H4869" display="ABC transporter, RND-adapter-like protein"/>
-    <hyperlink ref="B222" location="'Genome Annotation'!H4933" display="Cell-division-associated, ABC-transporter-like signaling protein FtsX"/>
-    <hyperlink ref="B223:B226" location="'Genome Annotation'!H4944" display="Excinuclease ABC subunit B"/>
-    <hyperlink ref="B224" location="'Genome Annotation'!H4945" display="Excinuclease ABC subunit A"/>
-    <hyperlink ref="B225" location="'Genome Annotation'!H4946" display="Excinuclease ABC subunit A"/>
-    <hyperlink ref="B226" location="'Genome Annotation'!H4947" display="Excinuclease ABC subunit A"/>
-    <hyperlink ref="B227:B233" location="'Genome Annotation'!H5023" display="Branched-chain amino acid ABC transporter, substrate-binding protein LivJ (TC 3.A.1.4.1)"/>
-    <hyperlink ref="B228" location="'Genome Annotation'!H5024" display="Branched-chain amino acid ABC transporter, substrate-binding protein LivJ (TC 3.A.1.4.1)"/>
-    <hyperlink ref="B229" location="'Genome Annotation'!H5025" display="Branched-chain amino acid ABC transporter, substrate-binding protein LivJ (TC 3.A.1.4.1)"/>
-    <hyperlink ref="B230" location="'Genome Annotation'!H5026" display="ABC transporter, permease protein 1 (cluster 4, leucine/isoleucine/valine/benzoate)"/>
-    <hyperlink ref="B231" location="'Genome Annotation'!H5027" display="Branched-chain amino acid ABC transporter, permease protein LivM (TC 3.A.1.4.1)"/>
-    <hyperlink ref="B232" location="'Genome Annotation'!H5028" display="Branched-chain amino acid ABC transporter, ATP-binding protein LivG (TC 3.A.1.4.1)"/>
-    <hyperlink ref="B233" location="'Genome Annotation'!H5029" display="Branched-chain amino acid ABC transporter, ATP-binding protein LivF (TC 3.A.1.4.1)"/>
-    <hyperlink ref="B234:B238" location="'Genome Annotation'!H5069" display="Methionine ABC transporter ATP-binding protein"/>
-    <hyperlink ref="B235" location="'Genome Annotation'!H5070" display="Methionine ABC transporter permease protein"/>
-    <hyperlink ref="B236" location="'Genome Annotation'!H5071" display="Methionine ABC transporter permease protein"/>
-    <hyperlink ref="B237" location="'Genome Annotation'!H5072" display="Methionine ABC transporter substrate-binding protein"/>
-    <hyperlink ref="B238" location="'Genome Annotation'!H5073" display="Methionine ABC transporter substrate-binding protein"/>
-    <hyperlink ref="B239:B244" location="'Genome Annotation'!H5105" display="Branched-chain amino acid ABC transporter, substrate-binding protein LivJ (TC 3.A.1.4.1)"/>
-    <hyperlink ref="B240" location="'Genome Annotation'!H5106" display="Branched-chain amino acid ABC transporter, substrate-binding protein LivJ (TC 3.A.1.4.1)"/>
-    <hyperlink ref="B241" location="'Genome Annotation'!H5107" display="Branched-chain amino acid ABC transporter, permease protein LivH (TC 3.A.1.4.1)"/>
-    <hyperlink ref="B242" location="'Genome Annotation'!H5108" display="Branched-chain amino acid ABC transporter, permease protein LivM (TC 3.A.1.4.1)"/>
-    <hyperlink ref="B243" location="'Genome Annotation'!H5109" display="Branched-chain amino acid ABC transporter, ATP-binding protein LivG (TC 3.A.1.4.1)"/>
-    <hyperlink ref="B244" location="'Genome Annotation'!H5110" display="Branched-chain amino acid ABC transporter, ATP-binding protein LivF (TC 3.A.1.4.1)"/>
-    <hyperlink ref="B245" location="'Genome Annotation'!H5148" display="Vitamin B12 ABC transporter, substrate-binding protein BtuF"/>
-    <hyperlink ref="B246" location="'Genome Annotation'!H5281" display="ABC transporter, ATP-binding protein"/>
-    <hyperlink ref="C211" r:id="rId13" tooltip="Go to alignment for MULTISPECIES: carbohydrate ABC transporter permease [Geobacillus] &gt;gb|ARA98361.1| sugar ABC transporter permease [Geobacillus thermodenitrificans] &gt;gb|ARP44252.1| L-arabinose transport system permease protein AraQ [Geobacillus thermode"/>
-    <hyperlink ref="C218" r:id="rId14" tooltip="Go to alignment for MULTISPECIES: ABC transporter substrate-binding protein [Geobacillus] &gt;gb|ABO68471.1| ABC transporter substrate-binding protein [Geobacillus thermodenitrificans NG80-2] &gt;gb|ARP44186.1| putative sugar-binding periplasmic protein [Geobac"/>
-    <hyperlink ref="C95" r:id="rId15" tooltip="Go to alignment for MULTISPECIES: ABC transporter ATP-binding protein/permease [Geobacillus] &gt;gb|ATO36078.1| ABC transporter ATP-binding protein [Geobacillus thermodenitrificans] &gt;gb|EDY06763.1| ABC transporter-related protein [Geobacillus thermodenitrifi"/>
-    <hyperlink ref="C96" r:id="rId16" tooltip="Go to alignment for MULTISPECIES: ABC transporter ATP-binding protein [Geobacillus] &gt;gb|ATO36087.1| ABC transporter [Geobacillus thermodenitrificans] &gt;gb|EDY06771.1| ABC transporter-related protein [Geobacillus thermodenitrificans] &gt;gb|OQP11051.1| ABC tra"/>
-    <hyperlink ref="C93" r:id="rId17" tooltip="Go to alignment for ABC transporter ATP-binding protein [Geobacillus thermodenitrificans] &gt;gb|ARP42631.1| putative ABC transporter ATP-binding protein YdbJ [Geobacillus thermodenitrificans]"/>
-    <hyperlink ref="C94" r:id="rId18" tooltip="Go to alignment for MULTISPECIES: ABC transporter ATP-binding protein/permease [Geobacillus] &gt;gb|ABO66848.1| ABC transporter ATP-binding protein [Geobacillus thermodenitrificans NG80-2] &gt;gb|ARP42614.1| putative ABC transporter ATP-binding protein [Geobaci"/>
-    <hyperlink ref="C97" r:id="rId19" tooltip="Go to alignment for ABC transporter ATP-binding protein [Geobacillus thermodenitrificans] &gt;gb|ARA96897.1| ABC transporter ATP-binding protein [Geobacillus thermodenitrificans] &gt;gb|EDY06870.1| ABC transporter-related protein [Geobacillus thermodenitrifican"/>
-    <hyperlink ref="C103" r:id="rId20" tooltip="Go to alignment for ABC-2 family transporter protein [Geobacillus sp. MR] &gt;gb|NNU85629.1| multidrug transporter [Geobacillus sp. MR]"/>
-    <hyperlink ref="C104" r:id="rId21" tooltip="Go to alignment for ABC-2 family transporter protein [Geobacillus thermodenitrificans] &gt;gb|PJW20497.1| multidrug ABC transporter permease [Geobacillus thermodenitrificans] &gt;gb|PTR48182.1| multidrug ABC transporter permease [Geobacillus thermodenitrificans"/>
-    <hyperlink ref="C46" r:id="rId22" tooltip="Go to alignment for MULTISPECIES: ABC transporter ATP-binding protein [Geobacillus] &gt;gb|ARA99483.1| bacitracin ABC transporter ATP-binding protein [Geobacillus thermodenitrificans] &gt;gb|ARP43097.1| putative ABC transporter ATP-binding protein YcbN [Geobaci"/>
-    <hyperlink ref="F209" r:id="rId23"/>
-    <hyperlink ref="F210" r:id="rId24"/>
-    <hyperlink ref="F218" r:id="rId25"/>
-    <hyperlink ref="F93" r:id="rId26"/>
-    <hyperlink ref="F25" r:id="rId27"/>
-    <hyperlink ref="F26" r:id="rId28"/>
-    <hyperlink ref="F27" r:id="rId29"/>
-    <hyperlink ref="F28" r:id="rId30"/>
-    <hyperlink ref="F29" r:id="rId31"/>
-    <hyperlink ref="F30" r:id="rId32"/>
-    <hyperlink ref="F29:F30" r:id="rId33" display="Uniprot"/>
-    <hyperlink ref="F31" r:id="rId34"/>
-    <hyperlink ref="F32" r:id="rId35"/>
-    <hyperlink ref="F33" r:id="rId36"/>
-    <hyperlink ref="G33" r:id="rId37" display=" Uniprot BtuD"/>
-    <hyperlink ref="F34" r:id="rId38"/>
-    <hyperlink ref="F35" r:id="rId39"/>
-    <hyperlink ref="F36" r:id="rId40"/>
-    <hyperlink ref="F50" r:id="rId41"/>
-    <hyperlink ref="F51:F52" r:id="rId42" display="Uniprot"/>
-    <hyperlink ref="F53" r:id="rId43"/>
-    <hyperlink ref="F54" r:id="rId44"/>
-    <hyperlink ref="F55" r:id="rId45"/>
-    <hyperlink ref="F56" r:id="rId46"/>
-    <hyperlink ref="F57" r:id="rId47"/>
-    <hyperlink ref="F58" r:id="rId48"/>
-    <hyperlink ref="F59" r:id="rId49"/>
-    <hyperlink ref="F60" r:id="rId50"/>
-    <hyperlink ref="F61" r:id="rId51"/>
-    <hyperlink ref="F62" r:id="rId52"/>
-    <hyperlink ref="F63" r:id="rId53"/>
-    <hyperlink ref="F64" r:id="rId54"/>
-    <hyperlink ref="F69" r:id="rId55"/>
-    <hyperlink ref="F70" r:id="rId56"/>
-    <hyperlink ref="F71" r:id="rId57"/>
-    <hyperlink ref="F72" r:id="rId58"/>
-    <hyperlink ref="E73" r:id="rId59" display="https://www.uniprot.org/citations/20693325"/>
-    <hyperlink ref="F73" r:id="rId60"/>
-    <hyperlink ref="E74" r:id="rId61" display="https://www.uniprot.org/citations/20693325"/>
-    <hyperlink ref="F74" r:id="rId62"/>
-    <hyperlink ref="E75" r:id="rId63" display="https://www.uniprot.org/citations/20693325"/>
-    <hyperlink ref="F75" r:id="rId64"/>
-    <hyperlink ref="E91" r:id="rId65" display="https://www.ebi.ac.uk/QuickGO/term/GO:0015556"/>
-    <hyperlink ref="F91" r:id="rId66"/>
-    <hyperlink ref="F94" r:id="rId67"/>
-    <hyperlink ref="F95" r:id="rId68"/>
-    <hyperlink ref="F6" r:id="rId69"/>
-    <hyperlink ref="F14" r:id="rId70"/>
-    <hyperlink ref="F15" r:id="rId71"/>
-    <hyperlink ref="F16" r:id="rId72"/>
-    <hyperlink ref="F17" r:id="rId73"/>
-    <hyperlink ref="F18" r:id="rId74"/>
-    <hyperlink ref="F19" r:id="rId75"/>
-    <hyperlink ref="F22" r:id="rId76"/>
-    <hyperlink ref="F20" r:id="rId77"/>
-    <hyperlink ref="F21" r:id="rId78"/>
-    <hyperlink ref="F24" r:id="rId79"/>
-    <hyperlink ref="F23" r:id="rId80"/>
-    <hyperlink ref="F41" r:id="rId81"/>
-    <hyperlink ref="F42" r:id="rId82"/>
-    <hyperlink ref="F43" r:id="rId83"/>
-    <hyperlink ref="E48" r:id="rId84" display="https://www.ebi.ac.uk/QuickGO/term/GO:0004252"/>
-    <hyperlink ref="F48" r:id="rId85"/>
-    <hyperlink ref="E90" r:id="rId86" display="https://www.ebi.ac.uk/QuickGO/term/GO:0015556"/>
-    <hyperlink ref="F90" r:id="rId87"/>
-    <hyperlink ref="F115" r:id="rId88"/>
-    <hyperlink ref="F116" r:id="rId89"/>
-    <hyperlink ref="F117" r:id="rId90"/>
-    <hyperlink ref="F118" r:id="rId91"/>
-    <hyperlink ref="F119" r:id="rId92"/>
-    <hyperlink ref="F120" r:id="rId93"/>
-    <hyperlink ref="C128" r:id="rId94" tooltip="Go to alignment for MULTISPECIES: heme ABC exporter ATP-binding protein CcmA [Geobacillus] &gt;gb|ARP41965.1| putative ABC transporter ATP-binding protein YbhF [Geobacillus thermodenitrificans] &gt;gb|ATO36680.1| heme ABC exporter, ATP-binding protein CcmA [Geo"/>
-    <hyperlink ref="C127" r:id="rId95" tooltip="Go to alignment for MULTISPECIES: ABC transporter permease [Geobacillus] &gt;gb|ARA97364.1| ABC transporter permease [Geobacillus thermodenitrificans] &gt;gb|ARP41966.1| Inner membrane transport permease YbhR [Geobacillus thermodenitrificans] &gt;gb|ATO36679.1| AB"/>
-    <hyperlink ref="C137" r:id="rId96" tooltip="Go to alignment for MULTISPECIES: ATP-binding cassette domain-containing protein [Geobacillus] &gt;gb|ARA97416.1| daunorubicin/doxorubicin resistance ABC transporter ATP-binding protein DrrA [Geobacillus thermodenitrificans] &gt;gb|EDY07478.1| daunorubicin resi"/>
-    <hyperlink ref="C138" r:id="rId97" location="alnHdr_WP_100660350" tooltip="Go to alignment for ATP-binding cassette domain-containing protein [Geobacillus thermodenitrificans] &gt;gb|PJW21447.1| daunorubicin/doxorubicin resistance ABC transporter ATP-binding protein DrrA [Geobacillus thermodenitrificans]" display="https://blast.ncbi.nlm.nih.gov/Blast.cgi - alnHdr_WP_100660350"/>
-    <hyperlink ref="C139" r:id="rId98"/>
-    <hyperlink ref="C140" r:id="rId99"/>
-    <hyperlink ref="C37" r:id="rId100"/>
-    <hyperlink ref="C38" r:id="rId101"/>
-    <hyperlink ref="C39" r:id="rId102"/>
-    <hyperlink ref="C47" r:id="rId103"/>
-    <hyperlink ref="C49" r:id="rId104"/>
-    <hyperlink ref="C44" r:id="rId105"/>
-    <hyperlink ref="C45" r:id="rId106"/>
-    <hyperlink ref="C65" r:id="rId107"/>
-    <hyperlink ref="C68" r:id="rId108"/>
-    <hyperlink ref="C76" r:id="rId109"/>
-    <hyperlink ref="C77" r:id="rId110"/>
-    <hyperlink ref="C78" r:id="rId111"/>
-    <hyperlink ref="C79" r:id="rId112"/>
-    <hyperlink ref="C80" r:id="rId113"/>
-    <hyperlink ref="C81" r:id="rId114"/>
-    <hyperlink ref="C82" r:id="rId115"/>
-    <hyperlink ref="C40" r:id="rId116"/>
-    <hyperlink ref="C83" r:id="rId117"/>
-    <hyperlink ref="C84" r:id="rId118"/>
-    <hyperlink ref="C85" r:id="rId119"/>
-    <hyperlink ref="C86" r:id="rId120"/>
-    <hyperlink ref="C87" r:id="rId121"/>
-    <hyperlink ref="C88" r:id="rId122"/>
-    <hyperlink ref="C89" r:id="rId123"/>
-    <hyperlink ref="C92" r:id="rId124"/>
-    <hyperlink ref="C98" r:id="rId125"/>
-    <hyperlink ref="C99" r:id="rId126"/>
-    <hyperlink ref="C100" r:id="rId127"/>
-    <hyperlink ref="C101" r:id="rId128"/>
-    <hyperlink ref="C102" r:id="rId129"/>
-    <hyperlink ref="C105" r:id="rId130"/>
-    <hyperlink ref="F141" r:id="rId131"/>
-    <hyperlink ref="F142:F145" r:id="rId132" display="Uniprot"/>
-    <hyperlink ref="F153" r:id="rId133"/>
-    <hyperlink ref="F149:F152" r:id="rId134" display="Uniprot"/>
-    <hyperlink ref="F148" r:id="rId135"/>
-    <hyperlink ref="F149" r:id="rId136"/>
-    <hyperlink ref="F150" r:id="rId137"/>
-    <hyperlink ref="F151" r:id="rId138"/>
-    <hyperlink ref="F152" r:id="rId139"/>
-    <hyperlink ref="F154" r:id="rId140"/>
-    <hyperlink ref="F155" r:id="rId141"/>
-    <hyperlink ref="F159" r:id="rId142"/>
-    <hyperlink ref="F160" r:id="rId143"/>
-    <hyperlink ref="F163" r:id="rId144"/>
-    <hyperlink ref="F167" r:id="rId145"/>
-    <hyperlink ref="F168" r:id="rId146"/>
-    <hyperlink ref="F169" r:id="rId147"/>
-    <hyperlink ref="F170" r:id="rId148"/>
-    <hyperlink ref="F171" r:id="rId149"/>
-    <hyperlink ref="F172" r:id="rId150"/>
-    <hyperlink ref="F173" r:id="rId151"/>
-    <hyperlink ref="F174" r:id="rId152"/>
-    <hyperlink ref="F179" r:id="rId153"/>
-    <hyperlink ref="F180" r:id="rId154"/>
-    <hyperlink ref="F185" r:id="rId155"/>
-    <hyperlink ref="F189" r:id="rId156"/>
-    <hyperlink ref="F190" r:id="rId157"/>
-    <hyperlink ref="F191" r:id="rId158"/>
-    <hyperlink ref="F194" r:id="rId159"/>
-    <hyperlink ref="F195" r:id="rId160"/>
-    <hyperlink ref="C193" r:id="rId161"/>
-    <hyperlink ref="C194" r:id="rId162"/>
-    <hyperlink ref="C195" r:id="rId163"/>
-    <hyperlink ref="F197" r:id="rId164"/>
-    <hyperlink ref="F198" r:id="rId165"/>
-    <hyperlink ref="F199" r:id="rId166"/>
-    <hyperlink ref="F200" r:id="rId167"/>
-    <hyperlink ref="F201" r:id="rId168"/>
-    <hyperlink ref="F206" r:id="rId169"/>
-    <hyperlink ref="F207" r:id="rId170"/>
-    <hyperlink ref="F208" r:id="rId171"/>
-    <hyperlink ref="F212" r:id="rId172"/>
-    <hyperlink ref="F213" r:id="rId173"/>
-    <hyperlink ref="F214" r:id="rId174"/>
-    <hyperlink ref="F215" r:id="rId175"/>
-    <hyperlink ref="F216" r:id="rId176"/>
-    <hyperlink ref="F227" r:id="rId177"/>
-    <hyperlink ref="F228:F229" r:id="rId178" display="Uniprot"/>
-    <hyperlink ref="F231" r:id="rId179"/>
-    <hyperlink ref="F232" r:id="rId180"/>
-    <hyperlink ref="F233" r:id="rId181"/>
-    <hyperlink ref="F239" r:id="rId182"/>
-    <hyperlink ref="F240" r:id="rId183"/>
-    <hyperlink ref="F241" r:id="rId184"/>
-    <hyperlink ref="F242" r:id="rId185"/>
-    <hyperlink ref="F244" r:id="rId186"/>
-    <hyperlink ref="F243" r:id="rId187"/>
-    <hyperlink ref="F245" r:id="rId188"/>
-    <hyperlink ref="C106" r:id="rId189"/>
-    <hyperlink ref="C107" r:id="rId190"/>
-    <hyperlink ref="C108" r:id="rId191"/>
-    <hyperlink ref="C109" r:id="rId192"/>
-    <hyperlink ref="C110" r:id="rId193"/>
-    <hyperlink ref="C111" r:id="rId194"/>
-    <hyperlink ref="C112" r:id="rId195"/>
-    <hyperlink ref="C113" r:id="rId196"/>
-    <hyperlink ref="C114" r:id="rId197"/>
-    <hyperlink ref="C121" r:id="rId198"/>
-    <hyperlink ref="C122" r:id="rId199"/>
-    <hyperlink ref="C123" r:id="rId200"/>
-    <hyperlink ref="C124" r:id="rId201"/>
-    <hyperlink ref="C125" r:id="rId202"/>
-    <hyperlink ref="C126" r:id="rId203"/>
-    <hyperlink ref="C129" r:id="rId204"/>
-    <hyperlink ref="C130" r:id="rId205"/>
-    <hyperlink ref="C131" r:id="rId206"/>
-    <hyperlink ref="C132" r:id="rId207"/>
-    <hyperlink ref="C133" r:id="rId208"/>
-    <hyperlink ref="C134" r:id="rId209"/>
-    <hyperlink ref="C135" r:id="rId210"/>
-    <hyperlink ref="C136" r:id="rId211"/>
-    <hyperlink ref="C141" r:id="rId212"/>
-    <hyperlink ref="C142" r:id="rId213"/>
-    <hyperlink ref="C143" r:id="rId214"/>
-    <hyperlink ref="C144" r:id="rId215"/>
-    <hyperlink ref="C145" r:id="rId216"/>
-    <hyperlink ref="C146" r:id="rId217"/>
-    <hyperlink ref="C148" r:id="rId218"/>
-    <hyperlink ref="C156" r:id="rId219"/>
-    <hyperlink ref="C157" r:id="rId220"/>
-    <hyperlink ref="C158" r:id="rId221"/>
-    <hyperlink ref="C159" r:id="rId222"/>
-    <hyperlink ref="C160" r:id="rId223"/>
-    <hyperlink ref="C161" r:id="rId224"/>
-    <hyperlink ref="C162" r:id="rId225"/>
-    <hyperlink ref="C164" r:id="rId226"/>
-    <hyperlink ref="C165" r:id="rId227"/>
-    <hyperlink ref="C166" r:id="rId228"/>
-    <hyperlink ref="C167" r:id="rId229"/>
-    <hyperlink ref="C168" r:id="rId230"/>
-    <hyperlink ref="C169" r:id="rId231"/>
-    <hyperlink ref="C170" r:id="rId232"/>
-    <hyperlink ref="C171" r:id="rId233"/>
-    <hyperlink ref="C172" r:id="rId234"/>
-    <hyperlink ref="C175" r:id="rId235"/>
-    <hyperlink ref="C176" r:id="rId236"/>
-    <hyperlink ref="C177" r:id="rId237"/>
-    <hyperlink ref="C178" r:id="rId238"/>
-    <hyperlink ref="C181" r:id="rId239"/>
-    <hyperlink ref="C182" r:id="rId240"/>
-    <hyperlink ref="C183" r:id="rId241"/>
-    <hyperlink ref="C184" r:id="rId242"/>
-    <hyperlink ref="C185" r:id="rId243"/>
-    <hyperlink ref="C186" r:id="rId244"/>
-    <hyperlink ref="C187" r:id="rId245"/>
-    <hyperlink ref="C188" r:id="rId246"/>
-    <hyperlink ref="C189" r:id="rId247"/>
-    <hyperlink ref="C190" r:id="rId248"/>
-    <hyperlink ref="C191" r:id="rId249"/>
-    <hyperlink ref="C192" r:id="rId250"/>
-    <hyperlink ref="C196" r:id="rId251"/>
-    <hyperlink ref="C200" r:id="rId252"/>
-    <hyperlink ref="C201" r:id="rId253"/>
-    <hyperlink ref="C202" r:id="rId254"/>
-    <hyperlink ref="C203" r:id="rId255"/>
-    <hyperlink ref="C204" r:id="rId256"/>
-    <hyperlink ref="C205" r:id="rId257"/>
-    <hyperlink ref="C214" r:id="rId258"/>
-    <hyperlink ref="C215" r:id="rId259"/>
-    <hyperlink ref="C216" r:id="rId260"/>
-    <hyperlink ref="C217" r:id="rId261"/>
-    <hyperlink ref="C219" r:id="rId262"/>
-    <hyperlink ref="C220" r:id="rId263"/>
-    <hyperlink ref="C221" r:id="rId264"/>
-    <hyperlink ref="C222" r:id="rId265"/>
-    <hyperlink ref="C223" r:id="rId266"/>
-    <hyperlink ref="F223" r:id="rId267"/>
-    <hyperlink ref="C224" r:id="rId268"/>
-    <hyperlink ref="F224" r:id="rId269"/>
-    <hyperlink ref="C225" r:id="rId270"/>
-    <hyperlink ref="F225" r:id="rId271"/>
-    <hyperlink ref="C226" r:id="rId272"/>
-    <hyperlink ref="F226" r:id="rId273"/>
-    <hyperlink ref="C227" r:id="rId274"/>
-    <hyperlink ref="C228" r:id="rId275"/>
-    <hyperlink ref="C229" r:id="rId276"/>
-    <hyperlink ref="C230" r:id="rId277"/>
-    <hyperlink ref="C231" r:id="rId278"/>
-    <hyperlink ref="C232" r:id="rId279"/>
-    <hyperlink ref="C233" r:id="rId280"/>
-    <hyperlink ref="C234" r:id="rId281"/>
-    <hyperlink ref="C235" r:id="rId282"/>
-    <hyperlink ref="C236" r:id="rId283"/>
-    <hyperlink ref="C237" r:id="rId284"/>
-    <hyperlink ref="C238" r:id="rId285"/>
-    <hyperlink ref="C239" r:id="rId286"/>
-    <hyperlink ref="C240" r:id="rId287"/>
-    <hyperlink ref="C241" r:id="rId288"/>
-    <hyperlink ref="C242" r:id="rId289"/>
-    <hyperlink ref="C243" r:id="rId290"/>
-    <hyperlink ref="C244" r:id="rId291"/>
-    <hyperlink ref="C245" r:id="rId292"/>
-    <hyperlink ref="C246" r:id="rId293"/>
+    <hyperlink ref="B6" location="'Genome Annotation'!H93" display="Zinc ABC transporter, substrate-binding protein ZnuA" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C6" r:id="rId1" tooltip="Go to alignment for MULTISPECIES: metal ABC transporter substrate-binding protein [Geobacillus] &gt;gb|ABO68109.1| High-affinity zinc uptake system protein ZnuA [Geobacillus thermodenitrificans NG80-2] &gt;gb|ARA98737.1| adhesin [Geobacillus thermodenitrificans" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B7" location="'Genome Annotation'!H104" display="ABC transporter, permease protein (cluster 10, nitrate/sulfonate/bicarbonate)" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C7" r:id="rId2" display=" _x0009_MULTISPECIES: ABC transporter permease [Geobacillus]" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B8" location="'Genome Annotation'!H105" display="ABC transporter, ATP-binding protein (cluster 1, maltose/g3p/polyamine/iron); ABC transporter, ATP-binding protein (cluster 10, nitrate/sulfonate/bicarbonate)" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="C8" r:id="rId3" tooltip="Go to alignment for MULTISPECIES: ABC transporter ATP-binding protein [Geobacillus] &gt;gb|ABO68100.1| Putative transporter [Geobacillus thermodenitrificans NG80-2] &gt;gb|ARP43864.1| putative ABC transporter ATP-binding protein [Geobacillus thermodenitrificans" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="B9" location="'Genome Annotation'!H106" display="ABC transporter, ATP-binding protein (cluster 1, maltose/g3p/polyamine/iron); ABC transporter, ATP-binding protein (cluster 10, nitrate/sulfonate/bicarbonate)" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId4" tooltip="Go to alignment for MULTISPECIES: ABC transporter ATP-binding protein [Geobacillus] &gt;gb|ABO68100.1| Putative transporter [Geobacillus thermodenitrificans NG80-2] &gt;gb|ARP43864.1| putative ABC transporter ATP-binding protein [Geobacillus thermodenitrificans" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="B10" location="'Genome Annotation'!H107" display="ABC transporter, ATP-binding protein (cluster 1, maltose/g3p/polyamine/iron); ABC transporter, ATP-binding protein (cluster 10, nitrate/sulfonate/bicarbonate)" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="C10" r:id="rId5" tooltip="Go to alignment for ABC transporter ATP-binding protein [Geobacillus thermodenitrificans] &gt;gb|ARA98745.1| spermidine/putrescine ABC transporter ATP-binding protein [Geobacillus thermodenitrificans]" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="B11" location="'Genome Annotation'!H108" display="ABC transporter, substrate-binding protein (cluster 10, nitrate/sulfonate/bicarbonate)" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="C11" r:id="rId6" tooltip="Go to alignment for MULTISPECIES: ABC transporter substrate-binding protein [Geobacillus] &gt;gb|NNU86489.1| ABC transporter substrate-binding protein [Geobacillus sp. MR] &gt;gb|PJW22406.1| hypothetical protein CV632_03555 [Geobacillus thermodenitrificans]" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="B12" location="'Genome Annotation'!H109" display="ABC transporter, substrate-binding protein (cluster 10, nitrate/sulfonate/bicarbonate)" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="C12" r:id="rId7" tooltip="Go to alignment for NMT1/THI5 like protein [Geobacillus sp. BCO2]" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="B13" location="'Genome Annotation'!H110" display="ABC transporter, substrate-binding protein (cluster 10, nitrate/sulfonate/bicarbonate)" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="C13" r:id="rId8" tooltip="Go to alignment for ABC transporter substrate-binding protein [Geobacillus thermodenitrificans] &gt;gb|EDY05297.1| ABC transporter substrate-binding protein [Geobacillus thermodenitrificans]" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="B14" location="'Genome Annotation'!H312" display="Molybdenum ABC transporter, substrate-binding protein ModA" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="C14" r:id="rId9" tooltip="Go to alignment for MULTISPECIES: molybdate ABC transporter substrate-binding protein [Geobacillus] &gt;gb|OQP11615.1| molybdate ABC transporter substrate-binding protein [Geobacillus sp. 47C-IIb] &gt;gb|PTR46061.1| molybdate ABC transporter substrate-binding p" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="B15" location="'Genome Annotation'!H338" display="Alkanesulfonate ABC transporter substrate-binding protein SsuA" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="B16" location="'Genome Annotation'!H339" display="Alkanesulfonate ABC transporter substrate-binding protein SsuA" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="B17" location="'ABC Transporters'!H340" display="Alkanesulfonate ABC transporter permease protein SsuC" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="B18" location="'ABC Transporters'!H341" display="Alkanesulfonate ABC transporter permease protein SsuC" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="B19" location="'ABC Transporters'!H342" display="Alkanesulfonate ABC transporter permease protein SsuC" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="B20" location="'ABC Transporters'!H343" display="Alkanesulfonate ABC transporter ATP-binding protein SsuB" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="B21" location="'ABC Transporters'!H344" display="Alkanesulfonate ABC transporter ATP-binding protein SsuB" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="B22" location="'ABC Transporters'!H345" display="Alkanesulfonate ABC transporter substrate-binding protein SsuA" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="C15" r:id="rId10" tooltip="Go to alignment for Putative sulfonate binding protein precursor [Geobacillus thermodenitrificans NG80-2]" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="B23" location="'Genome Annotation'!H619" display="Zinc ABC transporter, ATP-binding protein ZnuC" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="B24" location="'Genome Annotation'!H620" display="Zinc ABC transporter, permease protein ZnuB" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="B25" location="'Genome Annotation'!H632" display="Phosphate ABC transporter, substrate-binding protein PstS (TC 3.A.1.7.1)" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="B26" location="'Genome Annotation'!H633" display="Phosphate ABC transporter, permease protein PstC (TC 3.A.1.7.1)" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="B27" location="'ABC Transporters'!H634" display="Phosphate ABC transporter, permease protein PstA (TC 3.A.1.7.1)" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="B28" location="'Genome Annotation'!H635" display="Phosphate ABC transporter, permease protein PstA (TC 3.A.1.7.1)" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="B29" location="'Genome Annotation'!H636" display="Phosphate ABC transporter, ATP-binding protein PstB (TC 3.A.1.7.1)" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="B30" location="'Genome Annotation'!H886" display="Vitamin B12 ABC transporter, substrate-binding protein BtuF" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="B31" location="'Genome Annotation'!H887" display="Vitamin B12 ABC transporter, substrate-binding protein BtuF" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="B32" location="'Genome Annotation'!H888" display="Vitamin B12 ABC transporter, permease protein BtuC" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="B33" location="'Genome Annotation'!H889" display="Vitamin B12 ABC transporter, ATP-binding protein BtuD / Adenosylcobinamide amidohydrolase (EC 3.5.1.90)" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="B34" location="'Genome Annotation'!H1139" display="Oligopeptide ABC transporter, permease protein OppC (TC 3.A.1.5.1)" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="B35" location="'Genome Annotation'!H1140" display="Oligopeptide ABC transporter, permease protein OppB (TC 3.A.1.5.1)" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="B36" location="'Genome Annotation'!H1141" display="Oligopeptide ABC transporter, permease protein OppB (TC 3.A.1.5.1)" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="C34" r:id="rId11" tooltip="Go to alignment for ABC transporter permease subunit [Geobacillus thermodenitrificans] &gt;gb|EDY05593.1| binding-protein-dependent transport systems inner membrane component [Geobacillus thermodenitrificans]" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="B37" location="'Genome Annotation'!H1146" display="Hydroxymethylpyrimidine ABC transporter, ATPase component" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="B38" location="'Genome Annotation'!H1147" display="Hydroxymethylpyrimidine ABC transporter, ATPase component" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="B39" location="'Genome Annotation'!H1148" display="Hydroxymethylpyrimidine ABC transporter, transmembrane component" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="B40" location="'Genome Annotation'!H1149" display="Hydroxymethylpyrimidine ABC transporter, substrate-binding component" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="B41" location="'Genome Annotation'!H1171" display="Maltodextrin ABC transporter, substrate-binding protein MdxE" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="B42" location="'Genome Annotation'!H1172" display="Maltodextrin ABC transporter, permease protein MdxF" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="B43" location="'Genome Annotation'!H1173" display="Maltodextrin ABC transporter, permease protein MdxG" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="B44" location="'Genome Annotation'!H1254" display="ABC transporter, permease protein" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="B45" location="'Genome Annotation'!H1255" display="ABC transporter, permease protein" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="B46" location="'Genome Annotation'!H1256" display="Efflux ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="B47" location="'Genome Annotation'!H1297" display="ABC transporter, substrate-binding protein (cluster 15, trp?)" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="B48" location="'Genome Annotation'!H1298" display="Predicted ABC transporter for tryptophane, permease protein TrpY" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="B49" location="'Genome Annotation'!H1299" display="ABC transporter, ATP-binding protein (cluster 15, trp?)" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="B50" location="'Genome Annotation'!H1310" display="Glycerol-3-phosphate ABC transporter, ATP-binding protein UgpC (TC 3.A.1.1.3)" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="B51" location="'Genome Annotation'!H1311" display="Glycerol-3-phosphate ABC transporter, ATP-binding protein UgpC (TC 3.A.1.1.3)" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="B52" location="'Genome Annotation'!H1312" display="Glycerol-3-phosphate ABC transporter, ATP-binding protein UgpC (TC 3.A.1.1.3)" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="B53" location="'Genome Annotation'!H1313" display="Glycerol-3-phosphate ABC transporter, permease protein UgpA (TC 3.A.1.1.3)" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
+    <hyperlink ref="B54" location="'Genome Annotation'!H1314" display="Glycerol-3-phosphate ABC transporter, permease protein UgpE (TC 3.A.1.1.3)" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
+    <hyperlink ref="B55" location="'Genome Annotation'!H1315" display="Glycerol-3-phosphate ABC transporter, substrate-binding protein UgpB" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="B56" location="'Genome Annotation'!H1316" display="Glycerol-3-phosphate ABC transporter, substrate-binding protein UgpB" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="B57" location="'Genome Annotation'!H1435" display="Urea ABC transporter, substrate-binding protein UrtA" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
+    <hyperlink ref="B58" location="'Genome Annotation'!H1436" display="Urea ABC transporter, substrate-binding protein UrtA" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
+    <hyperlink ref="B59" location="'Genome Annotation'!H1437" display="Urea ABC transporter, permease protein UrtB" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
+    <hyperlink ref="B60" location="'Genome Annotation'!H1438" display="Urea ABC transporter, permease protein UrtB" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
+    <hyperlink ref="B61" location="'Genome Annotation'!H1439" display="Urea ABC transporter, permease protein UrtC" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
+    <hyperlink ref="B62" location="'Genome Annotation'!H1440" display="Urea ABC transporter, ATPase protein UrtD" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
+    <hyperlink ref="B63" location="'Genome Annotation'!H1441" display="Urea ABC transporter, ATPase protein UrtD" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
+    <hyperlink ref="B64" location="'Genome Annotation'!H1442" display="Urea ABC transporter, ATPase protein UrtE" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
+    <hyperlink ref="B65" location="'Genome Annotation'!H1473" display="Maltose/maltodextrin ABC transporter, substrate binding periplasmic protein MalE" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
+    <hyperlink ref="B66" location="'Genome Annotation'!H1477" display="Maltose/maltodextrin ABC transporter, substrate binding periplasmic protein MalE" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
+    <hyperlink ref="B67" location="'Genome Annotation'!H1479" display="putative sugar ABC transporter, permease protein" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
+    <hyperlink ref="C67" r:id="rId12" tooltip="Go to alignment for MULTISPECIES: carbohydrate ABC transporter permease [unclassified Geobacillus] &gt;gb|QNU31522.1| carbohydrate ABC transporter permease [Geobacillus sp. 47C-IIb] &gt;gb|RXS91429.1| carbohydrate ABC transporter permease [Geobacillus sp. PK12]" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
+    <hyperlink ref="B68" location="'Genome Annotation'!H1495" display="ABC transporter, substrate-binding protein (cluster 2, ribose/xylose/arabinose/galactose)" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
+    <hyperlink ref="B69" location="'Genome Annotation'!H1499" display="L-arabinose ABC transporter, substrate-binding protein AraF" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
+    <hyperlink ref="B70" location="'Genome Annotation'!H1500" display="L-arabinose ABC transporter, ATP-binding protein AraG" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
+    <hyperlink ref="B71" location="'Genome Annotation'!H1501" display="L-arabinose ABC transporter, permease protein AraH" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
+    <hyperlink ref="B72" location="'Genome Annotation'!H1502" display="L-arabinose ABC transporter, permease protein AraH" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
+    <hyperlink ref="B73" location="'Genome Annotation'!H1509" display="Alpha-arabinosides ABC transport system, substrate-binding protein AraN" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
+    <hyperlink ref="B74" location="'Genome Annotation'!H1510" display="Alpha-arabinosides ABC transport system, permease protein AraP" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
+    <hyperlink ref="B75" location="'Genome Annotation'!H1511" display="Alpha-arabinosides ABC transport system, permease protein AraQ" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
+    <hyperlink ref="B76" location="'Genome Annotation'!H1525" display="Xylose ABC transporter, substrate-binding component" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
+    <hyperlink ref="B77" location="'Genome Annotation'!H1526" display="ABC transporter, permease protein 1 (cluster 1, maltose/g3p/polyamine/iron)" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
+    <hyperlink ref="B78" location="'Genome Annotation'!H1527" display="ABC transporter, permease protein 1 (cluster 1, maltose/g3p/polyamine/iron)" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
+    <hyperlink ref="B79" location="'Genome Annotation'!H1528" display="Xylose ABC transporter, ATP-binding component" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
+    <hyperlink ref="B80" location="'Genome Annotation'!H1534" display="ABC transporter, substrate-binding protein (cluster 1, maltose/g3p/polyamine/iron)" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
+    <hyperlink ref="B81" location="'Genome Annotation'!H1535" display="ABC transporter, permease protein 1 (cluster 1, maltose/g3p/polyamine/iron)" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
+    <hyperlink ref="B82" location="'Genome Annotation'!H1536" display="ABC transporter, permease protein 2 (cluster 1, maltose/g3p/polyamine/iron)" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
+    <hyperlink ref="B83" location="'Genome Annotation'!H1886" display="ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
+    <hyperlink ref="B84" location="'Genome Annotation'!H1900" display="ABC transporter, substrate-binding protein (cluster 4, leucine/isoleucine/valine/benzoate)" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
+    <hyperlink ref="B85" location="'Genome Annotation'!H1901" display="ABC transporter, substrate-binding protein (cluster 4, leucine/isoleucine/valine/benzoate)" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
+    <hyperlink ref="B86" location="'Genome Annotation'!H1902" display="ABC transporter, ATP-binding protein 1 (cluster 4, leucine/isoleucine/valine/benzoate)" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
+    <hyperlink ref="B87" location="'Genome Annotation'!H1903" display="ABC transporter, permease protein 2 (cluster 4, leucine/isoleucine/valine/benzoate)" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
+    <hyperlink ref="B88" location="'Genome Annotation'!H1904" display="ABC transporter, permease protein 2 (cluster 4, leucine/isoleucine/valine/benzoate)" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
+    <hyperlink ref="B89" location="'Genome Annotation'!H1905" display="ABC transporter, permease protein 1 (cluster 4, leucine/isoleucine/valine/benzoate)" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
+    <hyperlink ref="B90" location="'Genome Annotation'!H1906" display="ABC transporter, permease protein 1 (cluster 4, leucine/isoleucine/valine/benzoate)" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
+    <hyperlink ref="B93" location="'Genome Annotation'!H1930" display="Efflux ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
+    <hyperlink ref="B94" location="'Genome Annotation'!H1953" display="Efflux ABC transporter, permease/ATP-binding protein YfiC" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
+    <hyperlink ref="B95" location="'Genome Annotation'!H1954" display="Efflux ABC transporter, permease/ATP-binding protein YfiB" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
+    <hyperlink ref="B96" location="'Genome Annotation'!H1965" display="Efflux ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
+    <hyperlink ref="B97" location="'Genome Annotation'!H2103" display="Efflux ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
+    <hyperlink ref="B91" location="'Genome Annotation'!H1928" display="ABC transporter permease YhcI" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
+    <hyperlink ref="B92" location="'Genome Annotation'!H1929" display="ABC transporter, permease protein" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
+    <hyperlink ref="B98" location="'Genome Annotation'!H2104" display="ABC transporter, permease protein" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
+    <hyperlink ref="B99" location="'Genome Annotation'!H2139" display="Methionine ABC transporter ATP-binding protein" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
+    <hyperlink ref="B100" location="'Genome Annotation'!H2140" display="Methionine ABC transporter ATP-binding protein" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
+    <hyperlink ref="B101" location="'Genome Annotation'!H2141" display="Methionine ABC transporter permease protein" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
+    <hyperlink ref="B102" location="'Genome Annotation'!H2142" display="Methionine ABC transporter substrate-binding protein" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
+    <hyperlink ref="B103" location="'Genome Annotation'!H2157" display="Efflux ABC transporter, permease protein" xr:uid="{00000000-0004-0000-0100-00006D000000}"/>
+    <hyperlink ref="B104" location="'Genome Annotation'!H2158" display="Efflux ABC transporter, permease protein" xr:uid="{00000000-0004-0000-0100-00006E000000}"/>
+    <hyperlink ref="B105" location="'Genome Annotation'!H2159" display="Efflux ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-00006F000000}"/>
+    <hyperlink ref="B106:B107" location="'Genome Annotation'!H2178" display="ABC-type Fe3+-siderophore transport system, ATPase component" xr:uid="{00000000-0004-0000-0100-000070000000}"/>
+    <hyperlink ref="B108:B110" location="'Genome Annotation'!H2178" display="ABC-type Fe3+-siderophore transport system, permease 2 component" xr:uid="{00000000-0004-0000-0100-000071000000}"/>
+    <hyperlink ref="B107" location="'Genome Annotation'!H2179" display="ABC-type Fe3+-siderophore transport system, permease 2 component" xr:uid="{00000000-0004-0000-0100-000072000000}"/>
+    <hyperlink ref="B108" location="'Genome Annotation'!H2180" display="ABC-type Fe3+-siderophore transport system, permease 2 component" xr:uid="{00000000-0004-0000-0100-000073000000}"/>
+    <hyperlink ref="B109" location="'Genome Annotation'!H2181" display="ABC-type Fe3+-siderophore transport system, permease component" xr:uid="{00000000-0004-0000-0100-000074000000}"/>
+    <hyperlink ref="B110" location="'Genome Annotation'!H2182" display="ABC-type Fe3+-siderophore transport system, periplasmic iron-binding component" xr:uid="{00000000-0004-0000-0100-000075000000}"/>
+    <hyperlink ref="B111:B114" location="'ABC Transporters'!H2259" display="Uncharacterized iron compound ABC uptake transporter, substrate-binding protein" xr:uid="{00000000-0004-0000-0100-000076000000}"/>
+    <hyperlink ref="B112" location="'Genome Annotation'!H2260" display="Uncharacterized iron compound ABC uptake transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-000077000000}"/>
+    <hyperlink ref="B113" location="'Genome Annotation'!H2261" display="Uncharacterized iron compound ABC uptake transporter, permease protein" xr:uid="{00000000-0004-0000-0100-000078000000}"/>
+    <hyperlink ref="B114" location="'Genome Annotation'!H2262" display="Uncharacterized iron compound ABC uptake transporter, permease protein" xr:uid="{00000000-0004-0000-0100-000079000000}"/>
+    <hyperlink ref="B111" location="'Genome Annotation'!H2259" display="Uncharacterized iron compound ABC uptake transporter, substrate-binding protein" xr:uid="{00000000-0004-0000-0100-00007A000000}"/>
+    <hyperlink ref="B115:B120" location="'Genome Annotation'!H2414" display="Efflux ABC transporter, permease/ATP-binding protein MdlB" xr:uid="{00000000-0004-0000-0100-00007B000000}"/>
+    <hyperlink ref="B116" location="'Genome Annotation'!H2415" display="Efflux ABC transporter, permease/ATP-binding protein MdlB" xr:uid="{00000000-0004-0000-0100-00007C000000}"/>
+    <hyperlink ref="B117" location="'Genome Annotation'!H2416" display="Efflux ABC transporter, permease/ATP-binding protein MdlB" xr:uid="{00000000-0004-0000-0100-00007D000000}"/>
+    <hyperlink ref="B118" location="'Genome Annotation'!H2417" display="Efflux ABC transporter, permease/ATP-binding protein MdlA" xr:uid="{00000000-0004-0000-0100-00007E000000}"/>
+    <hyperlink ref="B119" location="'Genome Annotation'!H2418" display="Efflux ABC transporter, permease/ATP-binding protein MdlA" xr:uid="{00000000-0004-0000-0100-00007F000000}"/>
+    <hyperlink ref="B120" location="'Genome Annotation'!H2419" display="Efflux ABC transporter, permease/ATP-binding protein MdlA" xr:uid="{00000000-0004-0000-0100-000080000000}"/>
+    <hyperlink ref="B121" location="'Genome Annotation'!H2484" display="Transcriptional regulator in cluster with unspecified monosaccharide ABC transport system" xr:uid="{00000000-0004-0000-0100-000081000000}"/>
+    <hyperlink ref="B122:B125" location="'Genome Annotation'!H2494" display="Purine nucleoside ABC transporter, permease protein 2" xr:uid="{00000000-0004-0000-0100-000082000000}"/>
+    <hyperlink ref="B123" location="'Genome Annotation'!H2495" display="Purine nucleoside ABC transporter, permease protein 1" xr:uid="{00000000-0004-0000-0100-000083000000}"/>
+    <hyperlink ref="B124" location="'Genome Annotation'!H2496" display="Purine nucleoside ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-000084000000}"/>
+    <hyperlink ref="B125" location="'Genome Annotation'!H2498" display="Purine nucleoside ABC transporter, substrate-binding protein" xr:uid="{00000000-0004-0000-0100-000085000000}"/>
+    <hyperlink ref="B126" location="'Genome Annotation'!H2677" display="ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-000086000000}"/>
+    <hyperlink ref="B127:B128" location="'Genome Annotation'!H2931" display="Efflux ABC transporter, permease protein" xr:uid="{00000000-0004-0000-0100-000087000000}"/>
+    <hyperlink ref="B128" location="'Genome Annotation'!H2932" display="Efflux ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-000088000000}"/>
+    <hyperlink ref="B129:B132" location="'Genome Annotation'!H2957" display="5-methylthioribose ABC transporter, substrate-binding protein" xr:uid="{00000000-0004-0000-0100-000089000000}"/>
+    <hyperlink ref="B130" location="'Genome Annotation'!H2958" display="5-methylthioribose ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-00008A000000}"/>
+    <hyperlink ref="B131" location="'Genome Annotation'!H2959" display="5-methylthioribose ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-00008B000000}"/>
+    <hyperlink ref="B132" location="'Genome Annotation'!H2960" display="5-methylthioribose ABC transporter, permease protein" xr:uid="{00000000-0004-0000-0100-00008C000000}"/>
+    <hyperlink ref="B133:B136" location="'Genome Annotation'!H2970" display="N-acetyl-D-glucosamine ABC transporter, permease protein 2" xr:uid="{00000000-0004-0000-0100-00008D000000}"/>
+    <hyperlink ref="B134" location="'Genome Annotation'!H2971" display="N-acetyl-D-glucosamine ABC transporter, permease protein 1" xr:uid="{00000000-0004-0000-0100-00008E000000}"/>
+    <hyperlink ref="B135" location="'Genome Annotation'!H2972" display="ABC transporter, substrate-binding protein (cluster 1, maltose/g3p/polyamine/iron)" xr:uid="{00000000-0004-0000-0100-00008F000000}"/>
+    <hyperlink ref="B136" location="'Genome Annotation'!H2973" display="ABC transporter, substrate-binding protein (cluster 1, maltose/g3p/polyamine/iron)" xr:uid="{00000000-0004-0000-0100-000090000000}"/>
+    <hyperlink ref="B137:B140" location="'Genome Annotation'!H3016" display="Efflux ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-000091000000}"/>
+    <hyperlink ref="B138" location="'Genome Annotation'!H3017" display="Efflux ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-000092000000}"/>
+    <hyperlink ref="B139" location="'Genome Annotation'!H3018" display="Efflux ABC transporter, permease protein" xr:uid="{00000000-0004-0000-0100-000093000000}"/>
+    <hyperlink ref="B140" location="'Genome Annotation'!H3019" display="Efflux ABC transporter, permease protein" xr:uid="{00000000-0004-0000-0100-000094000000}"/>
+    <hyperlink ref="B141:B146" location="'Genome Annotation'!H3137" display="Oligopeptide ABC transporter, ATP-binding protein OppF (TC 3.A.1.5.1)" xr:uid="{00000000-0004-0000-0100-000095000000}"/>
+    <hyperlink ref="B142" location="'Genome Annotation'!H3138" display="Oligopeptide ABC transporter, ATP-binding protein OppD (TC 3.A.1.5.1)" xr:uid="{00000000-0004-0000-0100-000096000000}"/>
+    <hyperlink ref="B143" location="'Genome Annotation'!H3139" display="Oligopeptide ABC transporter, ATP-binding protein OppD (TC 3.A.1.5.1)" xr:uid="{00000000-0004-0000-0100-000097000000}"/>
+    <hyperlink ref="B144" location="'Genome Annotation'!H3140" display="Oligopeptide ABC transporter, permease protein OppC (TC 3.A.1.5.1)" xr:uid="{00000000-0004-0000-0100-000098000000}"/>
+    <hyperlink ref="B145" location="'Genome Annotation'!H3141" display="Oligopeptide ABC transporter, permease protein OppB (TC 3.A.1.5.1)" xr:uid="{00000000-0004-0000-0100-000099000000}"/>
+    <hyperlink ref="B146" location="'Genome Annotation'!H3142" display="ABC transporter, substrate-binding protein (cluster 5, nickel/peptides/opines)" xr:uid="{00000000-0004-0000-0100-00009A000000}"/>
+    <hyperlink ref="B147" location="'Genome Annotation'!H3181" display="Molybdenum ABC transporter permease protein ModB" xr:uid="{00000000-0004-0000-0100-00009B000000}"/>
+    <hyperlink ref="B148" location="'Genome Annotation'!H3229" display="Spermidine/putrescine import ABC transporter substrate-binding protein PotD (TC 3.A.1.11.1)" xr:uid="{00000000-0004-0000-0100-00009C000000}"/>
+    <hyperlink ref="B149:B152" location="'Genome Annotation'!H3230" display="Spermidine/putrescine import ABC transporter permease protein PotC (TC 3.A.1.11.1)" xr:uid="{00000000-0004-0000-0100-00009D000000}"/>
+    <hyperlink ref="B150" location="'Genome Annotation'!H3231" display="Spermidine/putrescine import ABC transporter permease protein PotB (TC 3.A.1.11.1)" xr:uid="{00000000-0004-0000-0100-00009E000000}"/>
+    <hyperlink ref="B151" location="'Genome Annotation'!H3232" display="Spermidine/putrescine import ABC transporter ATP-binding protein PotA (TC 3.A.1.11.1)" xr:uid="{00000000-0004-0000-0100-00009F000000}"/>
+    <hyperlink ref="B152" location="'Genome Annotation'!H3233" display="Spermidine/putrescine import ABC transporter ATP-binding protein PotA (TC 3.A.1.11.1)" xr:uid="{00000000-0004-0000-0100-0000A0000000}"/>
+    <hyperlink ref="B153:B155" location="'Genome Annotation'!H3249" display="Maltodextrin ABC transporter, permease protein MdxG" xr:uid="{00000000-0004-0000-0100-0000A1000000}"/>
+    <hyperlink ref="B154" location="'Genome Annotation'!H3250" display="Maltodextrin ABC transporter, permease protein MdxF" xr:uid="{00000000-0004-0000-0100-0000A2000000}"/>
+    <hyperlink ref="B155" location="'Genome Annotation'!H3251" display="Maltodextrin ABC transporter, substrate-binding protein MdxE" xr:uid="{00000000-0004-0000-0100-0000A3000000}"/>
+    <hyperlink ref="B156:B158" location="'Genome Annotation'!H3297" display="ABC transporter, ATP-binding protein (cluster 15, trp?)" xr:uid="{00000000-0004-0000-0100-0000A4000000}"/>
+    <hyperlink ref="B157" location="'Genome Annotation'!H3298" display="ABC transporter, permease protein (cluster 15, trp?)" xr:uid="{00000000-0004-0000-0100-0000A5000000}"/>
+    <hyperlink ref="B158" location="'Genome Annotation'!H3299" display="ABC transporter, substrate-binding protein (cluster 15, trp?)" xr:uid="{00000000-0004-0000-0100-0000A6000000}"/>
+    <hyperlink ref="B159:B160" location="'Genome Annotation'!H3311" display="ABC transporter, permease protein EscB" xr:uid="{00000000-0004-0000-0100-0000A7000000}"/>
+    <hyperlink ref="B160" location="'Genome Annotation'!H3312" display="ABC transporter, ATP-binding protein EcsA" xr:uid="{00000000-0004-0000-0100-0000A8000000}"/>
+    <hyperlink ref="B161:B162" location="'Genome Annotation'!H3329" display="ABC-type Na+ efflux pump, permease component" xr:uid="{00000000-0004-0000-0100-0000A9000000}"/>
+    <hyperlink ref="B162" location="'Genome Annotation'!H3330" display="Efflux ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-0000AA000000}"/>
+    <hyperlink ref="B163" location="'Genome Annotation'!H3344" display="Maltodextrin ABC transporter, ATP-binding protein MsmX" xr:uid="{00000000-0004-0000-0100-0000AB000000}"/>
+    <hyperlink ref="B164:B166" location="'Genome Annotation'!H3452" display="Efflux ABC transporter, permease protein" xr:uid="{00000000-0004-0000-0100-0000AC000000}"/>
+    <hyperlink ref="B165" location="'Genome Annotation'!H3453" display="Efflux ABC transporter, permease protein" xr:uid="{00000000-0004-0000-0100-0000AD000000}"/>
+    <hyperlink ref="B166" location="'Genome Annotation'!H3454" display="Efflux ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-0000AE000000}"/>
+    <hyperlink ref="B167:B174" location="'Genome Annotation'!H3480" display="Dipeptide ABC transporter, permease protein DppC (TC 3.A.1.5.2)" xr:uid="{00000000-0004-0000-0100-0000AF000000}"/>
+    <hyperlink ref="B168" location="'Genome Annotation'!H3481" display="Dipeptide ABC transporter, permease protein DppC (TC 3.A.1.5.2)" xr:uid="{00000000-0004-0000-0100-0000B0000000}"/>
+    <hyperlink ref="B169" location="'Genome Annotation'!H3482" display="Dipeptide ABC transporter, permease protein DppB (TC 3.A.1.5.2)" xr:uid="{00000000-0004-0000-0100-0000B1000000}"/>
+    <hyperlink ref="B170" location="'Genome Annotation'!H3483" display="Dipeptide ABC transporter, substrate-binding protein DppA (TC 3.A.1.5.2)" xr:uid="{00000000-0004-0000-0100-0000B2000000}"/>
+    <hyperlink ref="B171" location="'Genome Annotation'!H3484" display="Oligopeptide ABC transporter, ATP-binding protein OppF (TC 3.A.1.5.1)" xr:uid="{00000000-0004-0000-0100-0000B3000000}"/>
+    <hyperlink ref="B172" location="'Genome Annotation'!H3485" display="Oligopeptide ABC transporter, ATP-binding protein OppD (TC 3.A.1.5.1)" xr:uid="{00000000-0004-0000-0100-0000B4000000}"/>
+    <hyperlink ref="B173" location="'Genome Annotation'!H3486" display="Efflux ABC transporter, permease/ATP-binding protein YgaD" xr:uid="{00000000-0004-0000-0100-0000B5000000}"/>
+    <hyperlink ref="B174" location="'Genome Annotation'!H3487" display="Efflux ABC transporter, permease/ATP-binding protein YgaD" xr:uid="{00000000-0004-0000-0100-0000B6000000}"/>
+    <hyperlink ref="B175:B178" location="'Genome Annotation'!H3716" display="ABC transporter-coupled two-component system, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-0000B7000000}"/>
+    <hyperlink ref="B176" location="'Genome Annotation'!H3717" display="ABC transporter-coupled two-component system, fused permease protein" xr:uid="{00000000-0004-0000-0100-0000B8000000}"/>
+    <hyperlink ref="B177" location="'Genome Annotation'!H3718" display="ABC transporter-coupled two-component system, LuxR family response regulator" xr:uid="{00000000-0004-0000-0100-0000B9000000}"/>
+    <hyperlink ref="B178" location="'Genome Annotation'!H3719" display="ABC transporter-coupled two-component system, signal transduction histidine kinase" xr:uid="{00000000-0004-0000-0100-0000BA000000}"/>
+    <hyperlink ref="B179" location="'Genome Annotation'!H3807" display="ABC transporter-like sensor and permease protein YxdM" xr:uid="{00000000-0004-0000-0100-0000BB000000}"/>
+    <hyperlink ref="B180" location="'Genome Annotation'!H3808" display="ABC transporter-like sensor ATP-binding protein YxdL" xr:uid="{00000000-0004-0000-0100-0000BC000000}"/>
+    <hyperlink ref="B181:B185" location="'Genome Annotation'!H3852" display="ABC transporter, substrate-binding protein (cluster 13, osmolytes)" xr:uid="{00000000-0004-0000-0100-0000BD000000}"/>
+    <hyperlink ref="B182" location="'Genome Annotation'!H3853" display="ABC transporter, substrate-binding protein (cluster 13, osmolytes)" xr:uid="{00000000-0004-0000-0100-0000BE000000}"/>
+    <hyperlink ref="B183" location="'Genome Annotation'!H3854" display="ABC transporter, ATP-binding protein (cluster 13, osmolytes)" xr:uid="{00000000-0004-0000-0100-0000BF000000}"/>
+    <hyperlink ref="B184" location="'Genome Annotation'!H3855" display="ABC transporter, permease protein (cluster 13, osmolytes)" xr:uid="{00000000-0004-0000-0100-0000C0000000}"/>
+    <hyperlink ref="B185" location="'Genome Annotation'!H3856" display="putative ABC transporter, ATP-binding protein MutF" xr:uid="{00000000-0004-0000-0100-0000C1000000}"/>
+    <hyperlink ref="B186:B187" location="'Genome Annotation'!H3857" display="Lantibiotic ABC transporter" xr:uid="{00000000-0004-0000-0100-0000C2000000}"/>
+    <hyperlink ref="B187" location="'Genome Annotation'!H3858" display="Lantibiotic ABC transporter" xr:uid="{00000000-0004-0000-0100-0000C3000000}"/>
+    <hyperlink ref="B188" location="'Genome Annotation'!H3950" display="Bis-ABC ATPase YheS" xr:uid="{00000000-0004-0000-0100-0000C4000000}"/>
+    <hyperlink ref="B189:B191" location="'Genome Annotation'!H4048" display="Oligopeptide ABC transporter, permease protein OppC (TC 3.A.1.5.1)" xr:uid="{00000000-0004-0000-0100-0000C5000000}"/>
+    <hyperlink ref="B190" location="'Genome Annotation'!H4049" display="Oligopeptide ABC transporter, permease protein OppB (TC 3.A.1.5.1)" xr:uid="{00000000-0004-0000-0100-0000C6000000}"/>
+    <hyperlink ref="B191" location="'Genome Annotation'!H4050" display="Oligopeptide ABC transporter, permease protein OppB (TC 3.A.1.5.1)" xr:uid="{00000000-0004-0000-0100-0000C7000000}"/>
+    <hyperlink ref="B192" location="'Genome Annotation'!H4057" display="ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-0000C8000000}"/>
+    <hyperlink ref="B193:B195" location="'Genome Annotation'!H4372" display="Efflux ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-0000C9000000}"/>
+    <hyperlink ref="B194" location="'Genome Annotation'!H4373" display="Export ABC transporter permease protein BA1794" xr:uid="{00000000-0004-0000-0100-0000CA000000}"/>
+    <hyperlink ref="B195" location="'Genome Annotation'!H4374" display="Export ABC transporter permease protein BA1795" xr:uid="{00000000-0004-0000-0100-0000CB000000}"/>
+    <hyperlink ref="B196:B199" location="'Genome Annotation'!H4403" display="ABC transporter, ATP-binding protein (cluster 3, basic aa/glutamine/opines)" xr:uid="{00000000-0004-0000-0100-0000CC000000}"/>
+    <hyperlink ref="B197" location="'Genome Annotation'!H4404" display="Glutamine ABC transporter, permease protein GlnP" xr:uid="{00000000-0004-0000-0100-0000CD000000}"/>
+    <hyperlink ref="B198" location="'Genome Annotation'!H4405" display="Glutamine ABC transporter, substrate-binding protein GlnH" xr:uid="{00000000-0004-0000-0100-0000CE000000}"/>
+    <hyperlink ref="B199" location="'Genome Annotation'!H4406" display="Glutamine ABC transporter, substrate-binding protein GlnH" xr:uid="{00000000-0004-0000-0100-0000CF000000}"/>
+    <hyperlink ref="B200:B201" location="'Genome Annotation'!H4552" display="Oligopeptide ABC transporter, ATP-binding protein OppD (TC 3.A.1.5.1)" xr:uid="{00000000-0004-0000-0100-0000D0000000}"/>
+    <hyperlink ref="B201" location="'Genome Annotation'!H4553" display="Oligopeptide ABC transporter, ATP-binding protein OppF (TC 3.A.1.5.1)" xr:uid="{00000000-0004-0000-0100-0000D1000000}"/>
+    <hyperlink ref="B202:B204" location="'Genome Annotation'!H4597" display="ABC transporter, substrate-binding protein (cluster 1, maltose/g3p/polyamine/iron)" xr:uid="{00000000-0004-0000-0100-0000D2000000}"/>
+    <hyperlink ref="B203" location="'Genome Annotation'!H4598" display="ABC transporter, substrate-binding protein (cluster 1, maltose/g3p/polyamine/iron)" xr:uid="{00000000-0004-0000-0100-0000D3000000}"/>
+    <hyperlink ref="B204" location="'Genome Annotation'!H4599" display="ABC transporter, permease protein 1 (cluster 1, maltose/g3p/polyamine/iron)" xr:uid="{00000000-0004-0000-0100-0000D4000000}"/>
+    <hyperlink ref="B205:B208" location="'Genome Annotation'!H4620" display="ABC transporter, substrate-binding protein (cluster 1, maltose/g3p/polyamine/iron)" xr:uid="{00000000-0004-0000-0100-0000D5000000}"/>
+    <hyperlink ref="B206" location="'Genome Annotation'!H4621" display="Spermidine/putrescine import ABC transporter ATP-binding protein PotA (TC 3.A.1.11.1)" xr:uid="{00000000-0004-0000-0100-0000D6000000}"/>
+    <hyperlink ref="B207" location="'Genome Annotation'!H4622" display="Spermidine/putrescine import ABC transporter permease protein PotB (TC 3.A.1.11.1)" xr:uid="{00000000-0004-0000-0100-0000D7000000}"/>
+    <hyperlink ref="B208" location="'Genome Annotation'!H4623" display="Spermidine/putrescine import ABC transporter permease protein PotC (TC 3.A.1.11.1)" xr:uid="{00000000-0004-0000-0100-0000D8000000}"/>
+    <hyperlink ref="B209:B211" location="'Genome Annotation'!H4658" display="Multiple sugar ABC transporter, substrate-binding protein MsmE" xr:uid="{00000000-0004-0000-0100-0000D9000000}"/>
+    <hyperlink ref="B210" location="'Genome Annotation'!H4659" display="Multiple sugar ABC transporter, permease protein MsmF" xr:uid="{00000000-0004-0000-0100-0000DA000000}"/>
+    <hyperlink ref="B211" location="'Genome Annotation'!H4660" display="Sugar ABC transporter, permease protein precursor" xr:uid="{00000000-0004-0000-0100-0000DB000000}"/>
+    <hyperlink ref="B212:B216" location="'Genome Annotation'!H4719" display="Ribose ABC transporter, ATP-binding protein RbsA (TC 3.A.1.2.1)" xr:uid="{00000000-0004-0000-0100-0000DC000000}"/>
+    <hyperlink ref="B213" location="'Genome Annotation'!H4720" display="Ribose ABC transporter, ATP-binding protein RbsA (TC 3.A.1.2.1)" xr:uid="{00000000-0004-0000-0100-0000DD000000}"/>
+    <hyperlink ref="B214" location="'Genome Annotation'!H4721" display="Ribose ABC transporter, permease protein RbsC (TC 3.A.1.2.1)" xr:uid="{00000000-0004-0000-0100-0000DE000000}"/>
+    <hyperlink ref="B215" location="'Genome Annotation'!H4722" display="Ribose ABC transporter, substrate-binding protein RbsB (TC 3.A.1.2.1)" xr:uid="{00000000-0004-0000-0100-0000DF000000}"/>
+    <hyperlink ref="B216" location="'Genome Annotation'!H4723" display="Ribose ABC transporter, substrate-binding protein RbsB (TC 3.A.1.2.1)" xr:uid="{00000000-0004-0000-0100-0000E0000000}"/>
+    <hyperlink ref="B217" location="'Genome Annotation'!H4763" display="Xylose ABC transporter, substrate-binding component" xr:uid="{00000000-0004-0000-0100-0000E1000000}"/>
+    <hyperlink ref="B218:B220" location="'Genome Annotation'!H4766" display="Predicted beta-glucoside-regulated ABC transport system, sugar binding component, COG1653" xr:uid="{00000000-0004-0000-0100-0000E2000000}"/>
+    <hyperlink ref="B219" location="'Genome Annotation'!H4767" display="Predicted beta-glucoside-regulated ABC transport system, permease component 1, COG1175" xr:uid="{00000000-0004-0000-0100-0000E3000000}"/>
+    <hyperlink ref="B220" location="'Genome Annotation'!H4768" display="Predicted beta-glucoside-regulated ABC transport system, permease component 2, COG0395" xr:uid="{00000000-0004-0000-0100-0000E4000000}"/>
+    <hyperlink ref="B221" location="'Genome Annotation'!H4869" display="ABC transporter, RND-adapter-like protein" xr:uid="{00000000-0004-0000-0100-0000E5000000}"/>
+    <hyperlink ref="B222" location="'Genome Annotation'!H4933" display="Cell-division-associated, ABC-transporter-like signaling protein FtsX" xr:uid="{00000000-0004-0000-0100-0000E6000000}"/>
+    <hyperlink ref="B223:B226" location="'Genome Annotation'!H4944" display="Excinuclease ABC subunit B" xr:uid="{00000000-0004-0000-0100-0000E7000000}"/>
+    <hyperlink ref="B224" location="'Genome Annotation'!H4945" display="Excinuclease ABC subunit A" xr:uid="{00000000-0004-0000-0100-0000E8000000}"/>
+    <hyperlink ref="B225" location="'Genome Annotation'!H4946" display="Excinuclease ABC subunit A" xr:uid="{00000000-0004-0000-0100-0000E9000000}"/>
+    <hyperlink ref="B226" location="'Genome Annotation'!H4947" display="Excinuclease ABC subunit A" xr:uid="{00000000-0004-0000-0100-0000EA000000}"/>
+    <hyperlink ref="B227:B233" location="'Genome Annotation'!H5023" display="Branched-chain amino acid ABC transporter, substrate-binding protein LivJ (TC 3.A.1.4.1)" xr:uid="{00000000-0004-0000-0100-0000EB000000}"/>
+    <hyperlink ref="B228" location="'Genome Annotation'!H5024" display="Branched-chain amino acid ABC transporter, substrate-binding protein LivJ (TC 3.A.1.4.1)" xr:uid="{00000000-0004-0000-0100-0000EC000000}"/>
+    <hyperlink ref="B229" location="'Genome Annotation'!H5025" display="Branched-chain amino acid ABC transporter, substrate-binding protein LivJ (TC 3.A.1.4.1)" xr:uid="{00000000-0004-0000-0100-0000ED000000}"/>
+    <hyperlink ref="B230" location="'Genome Annotation'!H5026" display="ABC transporter, permease protein 1 (cluster 4, leucine/isoleucine/valine/benzoate)" xr:uid="{00000000-0004-0000-0100-0000EE000000}"/>
+    <hyperlink ref="B231" location="'Genome Annotation'!H5027" display="Branched-chain amino acid ABC transporter, permease protein LivM (TC 3.A.1.4.1)" xr:uid="{00000000-0004-0000-0100-0000EF000000}"/>
+    <hyperlink ref="B232" location="'Genome Annotation'!H5028" display="Branched-chain amino acid ABC transporter, ATP-binding protein LivG (TC 3.A.1.4.1)" xr:uid="{00000000-0004-0000-0100-0000F0000000}"/>
+    <hyperlink ref="B233" location="'Genome Annotation'!H5029" display="Branched-chain amino acid ABC transporter, ATP-binding protein LivF (TC 3.A.1.4.1)" xr:uid="{00000000-0004-0000-0100-0000F1000000}"/>
+    <hyperlink ref="B234:B238" location="'Genome Annotation'!H5069" display="Methionine ABC transporter ATP-binding protein" xr:uid="{00000000-0004-0000-0100-0000F2000000}"/>
+    <hyperlink ref="B235" location="'Genome Annotation'!H5070" display="Methionine ABC transporter permease protein" xr:uid="{00000000-0004-0000-0100-0000F3000000}"/>
+    <hyperlink ref="B236" location="'Genome Annotation'!H5071" display="Methionine ABC transporter permease protein" xr:uid="{00000000-0004-0000-0100-0000F4000000}"/>
+    <hyperlink ref="B237" location="'Genome Annotation'!H5072" display="Methionine ABC transporter substrate-binding protein" xr:uid="{00000000-0004-0000-0100-0000F5000000}"/>
+    <hyperlink ref="B238" location="'Genome Annotation'!H5073" display="Methionine ABC transporter substrate-binding protein" xr:uid="{00000000-0004-0000-0100-0000F6000000}"/>
+    <hyperlink ref="B239:B244" location="'Genome Annotation'!H5105" display="Branched-chain amino acid ABC transporter, substrate-binding protein LivJ (TC 3.A.1.4.1)" xr:uid="{00000000-0004-0000-0100-0000F7000000}"/>
+    <hyperlink ref="B240" location="'Genome Annotation'!H5106" display="Branched-chain amino acid ABC transporter, substrate-binding protein LivJ (TC 3.A.1.4.1)" xr:uid="{00000000-0004-0000-0100-0000F8000000}"/>
+    <hyperlink ref="B241" location="'Genome Annotation'!H5107" display="Branched-chain amino acid ABC transporter, permease protein LivH (TC 3.A.1.4.1)" xr:uid="{00000000-0004-0000-0100-0000F9000000}"/>
+    <hyperlink ref="B242" location="'Genome Annotation'!H5108" display="Branched-chain amino acid ABC transporter, permease protein LivM (TC 3.A.1.4.1)" xr:uid="{00000000-0004-0000-0100-0000FA000000}"/>
+    <hyperlink ref="B243" location="'Genome Annotation'!H5109" display="Branched-chain amino acid ABC transporter, ATP-binding protein LivG (TC 3.A.1.4.1)" xr:uid="{00000000-0004-0000-0100-0000FB000000}"/>
+    <hyperlink ref="B244" location="'Genome Annotation'!H5110" display="Branched-chain amino acid ABC transporter, ATP-binding protein LivF (TC 3.A.1.4.1)" xr:uid="{00000000-0004-0000-0100-0000FC000000}"/>
+    <hyperlink ref="B245" location="'Genome Annotation'!H5148" display="Vitamin B12 ABC transporter, substrate-binding protein BtuF" xr:uid="{00000000-0004-0000-0100-0000FD000000}"/>
+    <hyperlink ref="B246" location="'Genome Annotation'!H5281" display="ABC transporter, ATP-binding protein" xr:uid="{00000000-0004-0000-0100-0000FE000000}"/>
+    <hyperlink ref="C211" r:id="rId13" tooltip="Go to alignment for MULTISPECIES: carbohydrate ABC transporter permease [Geobacillus] &gt;gb|ARA98361.1| sugar ABC transporter permease [Geobacillus thermodenitrificans] &gt;gb|ARP44252.1| L-arabinose transport system permease protein AraQ [Geobacillus thermode" xr:uid="{00000000-0004-0000-0100-0000FF000000}"/>
+    <hyperlink ref="C218" r:id="rId14" tooltip="Go to alignment for MULTISPECIES: ABC transporter substrate-binding protein [Geobacillus] &gt;gb|ABO68471.1| ABC transporter substrate-binding protein [Geobacillus thermodenitrificans NG80-2] &gt;gb|ARP44186.1| putative sugar-binding periplasmic protein [Geobac" xr:uid="{00000000-0004-0000-0100-000000010000}"/>
+    <hyperlink ref="C95" r:id="rId15" tooltip="Go to alignment for MULTISPECIES: ABC transporter ATP-binding protein/permease [Geobacillus] &gt;gb|ATO36078.1| ABC transporter ATP-binding protein [Geobacillus thermodenitrificans] &gt;gb|EDY06763.1| ABC transporter-related protein [Geobacillus thermodenitrifi" xr:uid="{00000000-0004-0000-0100-000001010000}"/>
+    <hyperlink ref="C96" r:id="rId16" tooltip="Go to alignment for MULTISPECIES: ABC transporter ATP-binding protein [Geobacillus] &gt;gb|ATO36087.1| ABC transporter [Geobacillus thermodenitrificans] &gt;gb|EDY06771.1| ABC transporter-related protein [Geobacillus thermodenitrificans] &gt;gb|OQP11051.1| ABC tra" xr:uid="{00000000-0004-0000-0100-000002010000}"/>
+    <hyperlink ref="C93" r:id="rId17" tooltip="Go to alignment for ABC transporter ATP-binding protein [Geobacillus thermodenitrificans] &gt;gb|ARP42631.1| putative ABC transporter ATP-binding protein YdbJ [Geobacillus thermodenitrificans]" xr:uid="{00000000-0004-0000-0100-000003010000}"/>
+    <hyperlink ref="C94" r:id="rId18" tooltip="Go to alignment for MULTISPECIES: ABC transporter ATP-binding protein/permease [Geobacillus] &gt;gb|ABO66848.1| ABC transporter ATP-binding protein [Geobacillus thermodenitrificans NG80-2] &gt;gb|ARP42614.1| putative ABC transporter ATP-binding protein [Geobaci" xr:uid="{00000000-0004-0000-0100-000004010000}"/>
+    <hyperlink ref="C97" r:id="rId19" tooltip="Go to alignment for ABC transporter ATP-binding protein [Geobacillus thermodenitrificans] &gt;gb|ARA96897.1| ABC transporter ATP-binding protein [Geobacillus thermodenitrificans] &gt;gb|EDY06870.1| ABC transporter-related protein [Geobacillus thermodenitrifican" xr:uid="{00000000-0004-0000-0100-000005010000}"/>
+    <hyperlink ref="C103" r:id="rId20" tooltip="Go to alignment for ABC-2 family transporter protein [Geobacillus sp. MR] &gt;gb|NNU85629.1| multidrug transporter [Geobacillus sp. MR]" xr:uid="{00000000-0004-0000-0100-000006010000}"/>
+    <hyperlink ref="C104" r:id="rId21" tooltip="Go to alignment for ABC-2 family transporter protein [Geobacillus thermodenitrificans] &gt;gb|PJW20497.1| multidrug ABC transporter permease [Geobacillus thermodenitrificans] &gt;gb|PTR48182.1| multidrug ABC transporter permease [Geobacillus thermodenitrificans" xr:uid="{00000000-0004-0000-0100-000007010000}"/>
+    <hyperlink ref="C46" r:id="rId22" tooltip="Go to alignment for MULTISPECIES: ABC transporter ATP-binding protein [Geobacillus] &gt;gb|ARA99483.1| bacitracin ABC transporter ATP-binding protein [Geobacillus thermodenitrificans] &gt;gb|ARP43097.1| putative ABC transporter ATP-binding protein YcbN [Geobaci" xr:uid="{00000000-0004-0000-0100-000008010000}"/>
+    <hyperlink ref="F209" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000009010000}"/>
+    <hyperlink ref="F210" r:id="rId24" xr:uid="{00000000-0004-0000-0100-00000A010000}"/>
+    <hyperlink ref="F218" r:id="rId25" xr:uid="{00000000-0004-0000-0100-00000B010000}"/>
+    <hyperlink ref="F93" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00000C010000}"/>
+    <hyperlink ref="F25" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00000D010000}"/>
+    <hyperlink ref="F26" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00000E010000}"/>
+    <hyperlink ref="F27" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00000F010000}"/>
+    <hyperlink ref="F28" r:id="rId30" xr:uid="{00000000-0004-0000-0100-000010010000}"/>
+    <hyperlink ref="F29" r:id="rId31" xr:uid="{00000000-0004-0000-0100-000011010000}"/>
+    <hyperlink ref="F30" r:id="rId32" xr:uid="{00000000-0004-0000-0100-000012010000}"/>
+    <hyperlink ref="F29:F30" r:id="rId33" display="Uniprot" xr:uid="{00000000-0004-0000-0100-000013010000}"/>
+    <hyperlink ref="F31" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000014010000}"/>
+    <hyperlink ref="F32" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000015010000}"/>
+    <hyperlink ref="F33" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000016010000}"/>
+    <hyperlink ref="G33" r:id="rId37" display=" Uniprot BtuD" xr:uid="{00000000-0004-0000-0100-000017010000}"/>
+    <hyperlink ref="F34" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000018010000}"/>
+    <hyperlink ref="F35" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000019010000}"/>
+    <hyperlink ref="F36" r:id="rId40" xr:uid="{00000000-0004-0000-0100-00001A010000}"/>
+    <hyperlink ref="F50" r:id="rId41" xr:uid="{00000000-0004-0000-0100-00001B010000}"/>
+    <hyperlink ref="F51:F52" r:id="rId42" display="Uniprot" xr:uid="{00000000-0004-0000-0100-00001C010000}"/>
+    <hyperlink ref="F53" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00001D010000}"/>
+    <hyperlink ref="F54" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00001E010000}"/>
+    <hyperlink ref="F55" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00001F010000}"/>
+    <hyperlink ref="F56" r:id="rId46" xr:uid="{00000000-0004-0000-0100-000020010000}"/>
+    <hyperlink ref="F57" r:id="rId47" xr:uid="{00000000-0004-0000-0100-000021010000}"/>
+    <hyperlink ref="F58" r:id="rId48" xr:uid="{00000000-0004-0000-0100-000022010000}"/>
+    <hyperlink ref="F59" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000023010000}"/>
+    <hyperlink ref="F60" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000024010000}"/>
+    <hyperlink ref="F61" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000025010000}"/>
+    <hyperlink ref="F62" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000026010000}"/>
+    <hyperlink ref="F63" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000027010000}"/>
+    <hyperlink ref="F64" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000028010000}"/>
+    <hyperlink ref="F69" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000029010000}"/>
+    <hyperlink ref="F70" r:id="rId56" xr:uid="{00000000-0004-0000-0100-00002A010000}"/>
+    <hyperlink ref="F71" r:id="rId57" xr:uid="{00000000-0004-0000-0100-00002B010000}"/>
+    <hyperlink ref="F72" r:id="rId58" xr:uid="{00000000-0004-0000-0100-00002C010000}"/>
+    <hyperlink ref="E73" r:id="rId59" display="https://www.uniprot.org/citations/20693325" xr:uid="{00000000-0004-0000-0100-00002D010000}"/>
+    <hyperlink ref="F73" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00002E010000}"/>
+    <hyperlink ref="E74" r:id="rId61" display="https://www.uniprot.org/citations/20693325" xr:uid="{00000000-0004-0000-0100-00002F010000}"/>
+    <hyperlink ref="F74" r:id="rId62" xr:uid="{00000000-0004-0000-0100-000030010000}"/>
+    <hyperlink ref="E75" r:id="rId63" display="https://www.uniprot.org/citations/20693325" xr:uid="{00000000-0004-0000-0100-000031010000}"/>
+    <hyperlink ref="F75" r:id="rId64" xr:uid="{00000000-0004-0000-0100-000032010000}"/>
+    <hyperlink ref="E91" r:id="rId65" display="https://www.ebi.ac.uk/QuickGO/term/GO:0015556" xr:uid="{00000000-0004-0000-0100-000033010000}"/>
+    <hyperlink ref="F91" r:id="rId66" xr:uid="{00000000-0004-0000-0100-000034010000}"/>
+    <hyperlink ref="F94" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000035010000}"/>
+    <hyperlink ref="F95" r:id="rId68" xr:uid="{00000000-0004-0000-0100-000036010000}"/>
+    <hyperlink ref="F6" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000037010000}"/>
+    <hyperlink ref="F14" r:id="rId70" xr:uid="{00000000-0004-0000-0100-000038010000}"/>
+    <hyperlink ref="F15" r:id="rId71" xr:uid="{00000000-0004-0000-0100-000039010000}"/>
+    <hyperlink ref="F16" r:id="rId72" xr:uid="{00000000-0004-0000-0100-00003A010000}"/>
+    <hyperlink ref="F17" r:id="rId73" xr:uid="{00000000-0004-0000-0100-00003B010000}"/>
+    <hyperlink ref="F18" r:id="rId74" xr:uid="{00000000-0004-0000-0100-00003C010000}"/>
+    <hyperlink ref="F19" r:id="rId75" xr:uid="{00000000-0004-0000-0100-00003D010000}"/>
+    <hyperlink ref="F22" r:id="rId76" xr:uid="{00000000-0004-0000-0100-00003E010000}"/>
+    <hyperlink ref="F20" r:id="rId77" xr:uid="{00000000-0004-0000-0100-00003F010000}"/>
+    <hyperlink ref="F21" r:id="rId78" xr:uid="{00000000-0004-0000-0100-000040010000}"/>
+    <hyperlink ref="F24" r:id="rId79" xr:uid="{00000000-0004-0000-0100-000041010000}"/>
+    <hyperlink ref="F23" r:id="rId80" xr:uid="{00000000-0004-0000-0100-000042010000}"/>
+    <hyperlink ref="F41" r:id="rId81" xr:uid="{00000000-0004-0000-0100-000043010000}"/>
+    <hyperlink ref="F42" r:id="rId82" xr:uid="{00000000-0004-0000-0100-000044010000}"/>
+    <hyperlink ref="F43" r:id="rId83" xr:uid="{00000000-0004-0000-0100-000045010000}"/>
+    <hyperlink ref="E48" r:id="rId84" display="https://www.ebi.ac.uk/QuickGO/term/GO:0004252" xr:uid="{00000000-0004-0000-0100-000046010000}"/>
+    <hyperlink ref="F48" r:id="rId85" xr:uid="{00000000-0004-0000-0100-000047010000}"/>
+    <hyperlink ref="E90" r:id="rId86" display="https://www.ebi.ac.uk/QuickGO/term/GO:0015556" xr:uid="{00000000-0004-0000-0100-000048010000}"/>
+    <hyperlink ref="F90" r:id="rId87" xr:uid="{00000000-0004-0000-0100-000049010000}"/>
+    <hyperlink ref="F115" r:id="rId88" xr:uid="{00000000-0004-0000-0100-00004A010000}"/>
+    <hyperlink ref="F116" r:id="rId89" xr:uid="{00000000-0004-0000-0100-00004B010000}"/>
+    <hyperlink ref="F117" r:id="rId90" xr:uid="{00000000-0004-0000-0100-00004C010000}"/>
+    <hyperlink ref="F118" r:id="rId91" xr:uid="{00000000-0004-0000-0100-00004D010000}"/>
+    <hyperlink ref="F119" r:id="rId92" xr:uid="{00000000-0004-0000-0100-00004E010000}"/>
+    <hyperlink ref="F120" r:id="rId93" xr:uid="{00000000-0004-0000-0100-00004F010000}"/>
+    <hyperlink ref="C128" r:id="rId94" tooltip="Go to alignment for MULTISPECIES: heme ABC exporter ATP-binding protein CcmA [Geobacillus] &gt;gb|ARP41965.1| putative ABC transporter ATP-binding protein YbhF [Geobacillus thermodenitrificans] &gt;gb|ATO36680.1| heme ABC exporter, ATP-binding protein CcmA [Geo" xr:uid="{00000000-0004-0000-0100-000050010000}"/>
+    <hyperlink ref="C127" r:id="rId95" tooltip="Go to alignment for MULTISPECIES: ABC transporter permease [Geobacillus] &gt;gb|ARA97364.1| ABC transporter permease [Geobacillus thermodenitrificans] &gt;gb|ARP41966.1| Inner membrane transport permease YbhR [Geobacillus thermodenitrificans] &gt;gb|ATO36679.1| AB" xr:uid="{00000000-0004-0000-0100-000051010000}"/>
+    <hyperlink ref="C137" r:id="rId96" tooltip="Go to alignment for MULTISPECIES: ATP-binding cassette domain-containing protein [Geobacillus] &gt;gb|ARA97416.1| daunorubicin/doxorubicin resistance ABC transporter ATP-binding protein DrrA [Geobacillus thermodenitrificans] &gt;gb|EDY07478.1| daunorubicin resi" xr:uid="{00000000-0004-0000-0100-000052010000}"/>
+    <hyperlink ref="C138" r:id="rId97" location="alnHdr_WP_100660350" tooltip="Go to alignment for ATP-binding cassette domain-containing protein [Geobacillus thermodenitrificans] &gt;gb|PJW21447.1| daunorubicin/doxorubicin resistance ABC transporter ATP-binding protein DrrA [Geobacillus thermodenitrificans]" display="https://blast.ncbi.nlm.nih.gov/Blast.cgi - alnHdr_WP_100660350" xr:uid="{00000000-0004-0000-0100-000053010000}"/>
+    <hyperlink ref="C139" r:id="rId98" xr:uid="{00000000-0004-0000-0100-000054010000}"/>
+    <hyperlink ref="C140" r:id="rId99" xr:uid="{00000000-0004-0000-0100-000055010000}"/>
+    <hyperlink ref="C37" r:id="rId100" xr:uid="{00000000-0004-0000-0100-000056010000}"/>
+    <hyperlink ref="C38" r:id="rId101" xr:uid="{00000000-0004-0000-0100-000057010000}"/>
+    <hyperlink ref="C39" r:id="rId102" xr:uid="{00000000-0004-0000-0100-000058010000}"/>
+    <hyperlink ref="C47" r:id="rId103" xr:uid="{00000000-0004-0000-0100-000059010000}"/>
+    <hyperlink ref="C49" r:id="rId104" xr:uid="{00000000-0004-0000-0100-00005A010000}"/>
+    <hyperlink ref="C44" r:id="rId105" xr:uid="{00000000-0004-0000-0100-00005B010000}"/>
+    <hyperlink ref="C45" r:id="rId106" xr:uid="{00000000-0004-0000-0100-00005C010000}"/>
+    <hyperlink ref="C65" r:id="rId107" xr:uid="{00000000-0004-0000-0100-00005D010000}"/>
+    <hyperlink ref="C68" r:id="rId108" xr:uid="{00000000-0004-0000-0100-00005E010000}"/>
+    <hyperlink ref="C76" r:id="rId109" xr:uid="{00000000-0004-0000-0100-00005F010000}"/>
+    <hyperlink ref="C77" r:id="rId110" xr:uid="{00000000-0004-0000-0100-000060010000}"/>
+    <hyperlink ref="C78" r:id="rId111" xr:uid="{00000000-0004-0000-0100-000061010000}"/>
+    <hyperlink ref="C79" r:id="rId112" xr:uid="{00000000-0004-0000-0100-000062010000}"/>
+    <hyperlink ref="C80" r:id="rId113" xr:uid="{00000000-0004-0000-0100-000063010000}"/>
+    <hyperlink ref="C81" r:id="rId114" xr:uid="{00000000-0004-0000-0100-000064010000}"/>
+    <hyperlink ref="C82" r:id="rId115" xr:uid="{00000000-0004-0000-0100-000065010000}"/>
+    <hyperlink ref="C40" r:id="rId116" xr:uid="{00000000-0004-0000-0100-000066010000}"/>
+    <hyperlink ref="C83" r:id="rId117" xr:uid="{00000000-0004-0000-0100-000067010000}"/>
+    <hyperlink ref="C84" r:id="rId118" xr:uid="{00000000-0004-0000-0100-000068010000}"/>
+    <hyperlink ref="C85" r:id="rId119" xr:uid="{00000000-0004-0000-0100-000069010000}"/>
+    <hyperlink ref="C86" r:id="rId120" xr:uid="{00000000-0004-0000-0100-00006A010000}"/>
+    <hyperlink ref="C87" r:id="rId121" xr:uid="{00000000-0004-0000-0100-00006B010000}"/>
+    <hyperlink ref="C88" r:id="rId122" xr:uid="{00000000-0004-0000-0100-00006C010000}"/>
+    <hyperlink ref="C89" r:id="rId123" xr:uid="{00000000-0004-0000-0100-00006D010000}"/>
+    <hyperlink ref="C92" r:id="rId124" xr:uid="{00000000-0004-0000-0100-00006E010000}"/>
+    <hyperlink ref="C98" r:id="rId125" xr:uid="{00000000-0004-0000-0100-00006F010000}"/>
+    <hyperlink ref="C99" r:id="rId126" xr:uid="{00000000-0004-0000-0100-000070010000}"/>
+    <hyperlink ref="C100" r:id="rId127" xr:uid="{00000000-0004-0000-0100-000071010000}"/>
+    <hyperlink ref="C101" r:id="rId128" xr:uid="{00000000-0004-0000-0100-000072010000}"/>
+    <hyperlink ref="C102" r:id="rId129" xr:uid="{00000000-0004-0000-0100-000073010000}"/>
+    <hyperlink ref="C105" r:id="rId130" xr:uid="{00000000-0004-0000-0100-000074010000}"/>
+    <hyperlink ref="F141" r:id="rId131" xr:uid="{00000000-0004-0000-0100-000075010000}"/>
+    <hyperlink ref="F142:F145" r:id="rId132" display="Uniprot" xr:uid="{00000000-0004-0000-0100-000076010000}"/>
+    <hyperlink ref="F153" r:id="rId133" xr:uid="{00000000-0004-0000-0100-000077010000}"/>
+    <hyperlink ref="F149:F152" r:id="rId134" display="Uniprot" xr:uid="{00000000-0004-0000-0100-000078010000}"/>
+    <hyperlink ref="F148" r:id="rId135" xr:uid="{00000000-0004-0000-0100-000079010000}"/>
+    <hyperlink ref="F149" r:id="rId136" xr:uid="{00000000-0004-0000-0100-00007A010000}"/>
+    <hyperlink ref="F150" r:id="rId137" xr:uid="{00000000-0004-0000-0100-00007B010000}"/>
+    <hyperlink ref="F151" r:id="rId138" xr:uid="{00000000-0004-0000-0100-00007C010000}"/>
+    <hyperlink ref="F152" r:id="rId139" xr:uid="{00000000-0004-0000-0100-00007D010000}"/>
+    <hyperlink ref="F154" r:id="rId140" xr:uid="{00000000-0004-0000-0100-00007E010000}"/>
+    <hyperlink ref="F155" r:id="rId141" xr:uid="{00000000-0004-0000-0100-00007F010000}"/>
+    <hyperlink ref="F159" r:id="rId142" xr:uid="{00000000-0004-0000-0100-000080010000}"/>
+    <hyperlink ref="F160" r:id="rId143" xr:uid="{00000000-0004-0000-0100-000081010000}"/>
+    <hyperlink ref="F163" r:id="rId144" xr:uid="{00000000-0004-0000-0100-000082010000}"/>
+    <hyperlink ref="F167" r:id="rId145" xr:uid="{00000000-0004-0000-0100-000083010000}"/>
+    <hyperlink ref="F168" r:id="rId146" xr:uid="{00000000-0004-0000-0100-000084010000}"/>
+    <hyperlink ref="F169" r:id="rId147" xr:uid="{00000000-0004-0000-0100-000085010000}"/>
+    <hyperlink ref="F170" r:id="rId148" xr:uid="{00000000-0004-0000-0100-000086010000}"/>
+    <hyperlink ref="F171" r:id="rId149" xr:uid="{00000000-0004-0000-0100-000087010000}"/>
+    <hyperlink ref="F172" r:id="rId150" xr:uid="{00000000-0004-0000-0100-000088010000}"/>
+    <hyperlink ref="F173" r:id="rId151" xr:uid="{00000000-0004-0000-0100-000089010000}"/>
+    <hyperlink ref="F174" r:id="rId152" xr:uid="{00000000-0004-0000-0100-00008A010000}"/>
+    <hyperlink ref="F179" r:id="rId153" xr:uid="{00000000-0004-0000-0100-00008B010000}"/>
+    <hyperlink ref="F180" r:id="rId154" xr:uid="{00000000-0004-0000-0100-00008C010000}"/>
+    <hyperlink ref="F185" r:id="rId155" xr:uid="{00000000-0004-0000-0100-00008D010000}"/>
+    <hyperlink ref="F189" r:id="rId156" xr:uid="{00000000-0004-0000-0100-00008E010000}"/>
+    <hyperlink ref="F190" r:id="rId157" xr:uid="{00000000-0004-0000-0100-00008F010000}"/>
+    <hyperlink ref="F191" r:id="rId158" xr:uid="{00000000-0004-0000-0100-000090010000}"/>
+    <hyperlink ref="F194" r:id="rId159" xr:uid="{00000000-0004-0000-0100-000091010000}"/>
+    <hyperlink ref="F195" r:id="rId160" xr:uid="{00000000-0004-0000-0100-000092010000}"/>
+    <hyperlink ref="C193" r:id="rId161" xr:uid="{00000000-0004-0000-0100-000093010000}"/>
+    <hyperlink ref="C194" r:id="rId162" xr:uid="{00000000-0004-0000-0100-000094010000}"/>
+    <hyperlink ref="C195" r:id="rId163" xr:uid="{00000000-0004-0000-0100-000095010000}"/>
+    <hyperlink ref="F197" r:id="rId164" xr:uid="{00000000-0004-0000-0100-000096010000}"/>
+    <hyperlink ref="F198" r:id="rId165" xr:uid="{00000000-0004-0000-0100-000097010000}"/>
+    <hyperlink ref="F199" r:id="rId166" xr:uid="{00000000-0004-0000-0100-000098010000}"/>
+    <hyperlink ref="F200" r:id="rId167" xr:uid="{00000000-0004-0000-0100-000099010000}"/>
+    <hyperlink ref="F201" r:id="rId168" xr:uid="{00000000-0004-0000-0100-00009A010000}"/>
+    <hyperlink ref="F206" r:id="rId169" xr:uid="{00000000-0004-0000-0100-00009B010000}"/>
+    <hyperlink ref="F207" r:id="rId170" xr:uid="{00000000-0004-0000-0100-00009C010000}"/>
+    <hyperlink ref="F208" r:id="rId171" xr:uid="{00000000-0004-0000-0100-00009D010000}"/>
+    <hyperlink ref="F212" r:id="rId172" xr:uid="{00000000-0004-0000-0100-00009E010000}"/>
+    <hyperlink ref="F213" r:id="rId173" xr:uid="{00000000-0004-0000-0100-00009F010000}"/>
+    <hyperlink ref="F214" r:id="rId174" xr:uid="{00000000-0004-0000-0100-0000A0010000}"/>
+    <hyperlink ref="F215" r:id="rId175" xr:uid="{00000000-0004-0000-0100-0000A1010000}"/>
+    <hyperlink ref="F216" r:id="rId176" xr:uid="{00000000-0004-0000-0100-0000A2010000}"/>
+    <hyperlink ref="F227" r:id="rId177" xr:uid="{00000000-0004-0000-0100-0000A3010000}"/>
+    <hyperlink ref="F228:F229" r:id="rId178" display="Uniprot" xr:uid="{00000000-0004-0000-0100-0000A4010000}"/>
+    <hyperlink ref="F231" r:id="rId179" xr:uid="{00000000-0004-0000-0100-0000A5010000}"/>
+    <hyperlink ref="F232" r:id="rId180" xr:uid="{00000000-0004-0000-0100-0000A6010000}"/>
+    <hyperlink ref="F233" r:id="rId181" xr:uid="{00000000-0004-0000-0100-0000A7010000}"/>
+    <hyperlink ref="F239" r:id="rId182" xr:uid="{00000000-0004-0000-0100-0000A8010000}"/>
+    <hyperlink ref="F240" r:id="rId183" xr:uid="{00000000-0004-0000-0100-0000A9010000}"/>
+    <hyperlink ref="F241" r:id="rId184" xr:uid="{00000000-0004-0000-0100-0000AA010000}"/>
+    <hyperlink ref="F242" r:id="rId185" xr:uid="{00000000-0004-0000-0100-0000AB010000}"/>
+    <hyperlink ref="F244" r:id="rId186" xr:uid="{00000000-0004-0000-0100-0000AC010000}"/>
+    <hyperlink ref="F243" r:id="rId187" xr:uid="{00000000-0004-0000-0100-0000AD010000}"/>
+    <hyperlink ref="F245" r:id="rId188" xr:uid="{00000000-0004-0000-0100-0000AE010000}"/>
+    <hyperlink ref="C106" r:id="rId189" xr:uid="{00000000-0004-0000-0100-0000AF010000}"/>
+    <hyperlink ref="C107" r:id="rId190" xr:uid="{00000000-0004-0000-0100-0000B0010000}"/>
+    <hyperlink ref="C108" r:id="rId191" xr:uid="{00000000-0004-0000-0100-0000B1010000}"/>
+    <hyperlink ref="C109" r:id="rId192" xr:uid="{00000000-0004-0000-0100-0000B2010000}"/>
+    <hyperlink ref="C110" r:id="rId193" xr:uid="{00000000-0004-0000-0100-0000B3010000}"/>
+    <hyperlink ref="C111" r:id="rId194" xr:uid="{00000000-0004-0000-0100-0000B4010000}"/>
+    <hyperlink ref="C112" r:id="rId195" xr:uid="{00000000-0004-0000-0100-0000B5010000}"/>
+    <hyperlink ref="C113" r:id="rId196" xr:uid="{00000000-0004-0000-0100-0000B6010000}"/>
+    <hyperlink ref="C114" r:id="rId197" xr:uid="{00000000-0004-0000-0100-0000B7010000}"/>
+    <hyperlink ref="C121" r:id="rId198" xr:uid="{00000000-0004-0000-0100-0000B8010000}"/>
+    <hyperlink ref="C122" r:id="rId199" xr:uid="{00000000-0004-0000-0100-0000B9010000}"/>
+    <hyperlink ref="C123" r:id="rId200" xr:uid="{00000000-0004-0000-0100-0000BA010000}"/>
+    <hyperlink ref="C124" r:id="rId201" xr:uid="{00000000-0004-0000-0100-0000BB010000}"/>
+    <hyperlink ref="C125" r:id="rId202" xr:uid="{00000000-0004-0000-0100-0000BC010000}"/>
+    <hyperlink ref="C126" r:id="rId203" xr:uid="{00000000-0004-0000-0100-0000BD010000}"/>
+    <hyperlink ref="C129" r:id="rId204" xr:uid="{00000000-0004-0000-0100-0000BE010000}"/>
+    <hyperlink ref="C130" r:id="rId205" xr:uid="{00000000-0004-0000-0100-0000BF010000}"/>
+    <hyperlink ref="C131" r:id="rId206" xr:uid="{00000000-0004-0000-0100-0000C0010000}"/>
+    <hyperlink ref="C132" r:id="rId207" xr:uid="{00000000-0004-0000-0100-0000C1010000}"/>
+    <hyperlink ref="C133" r:id="rId208" xr:uid="{00000000-0004-0000-0100-0000C2010000}"/>
+    <hyperlink ref="C134" r:id="rId209" xr:uid="{00000000-0004-0000-0100-0000C3010000}"/>
+    <hyperlink ref="C135" r:id="rId210" xr:uid="{00000000-0004-0000-0100-0000C4010000}"/>
+    <hyperlink ref="C136" r:id="rId211" xr:uid="{00000000-0004-0000-0100-0000C5010000}"/>
+    <hyperlink ref="C141" r:id="rId212" xr:uid="{00000000-0004-0000-0100-0000C6010000}"/>
+    <hyperlink ref="C142" r:id="rId213" xr:uid="{00000000-0004-0000-0100-0000C7010000}"/>
+    <hyperlink ref="C143" r:id="rId214" xr:uid="{00000000-0004-0000-0100-0000C8010000}"/>
+    <hyperlink ref="C144" r:id="rId215" xr:uid="{00000000-0004-0000-0100-0000C9010000}"/>
+    <hyperlink ref="C145" r:id="rId216" xr:uid="{00000000-0004-0000-0100-0000CA010000}"/>
+    <hyperlink ref="C146" r:id="rId217" xr:uid="{00000000-0004-0000-0100-0000CB010000}"/>
+    <hyperlink ref="C148" r:id="rId218" xr:uid="{00000000-0004-0000-0100-0000CC010000}"/>
+    <hyperlink ref="C156" r:id="rId219" xr:uid="{00000000-0004-0000-0100-0000CD010000}"/>
+    <hyperlink ref="C157" r:id="rId220" xr:uid="{00000000-0004-0000-0100-0000CE010000}"/>
+    <hyperlink ref="C158" r:id="rId221" xr:uid="{00000000-0004-0000-0100-0000CF010000}"/>
+    <hyperlink ref="C159" r:id="rId222" xr:uid="{00000000-0004-0000-0100-0000D0010000}"/>
+    <hyperlink ref="C160" r:id="rId223" xr:uid="{00000000-0004-0000-0100-0000D1010000}"/>
+    <hyperlink ref="C161" r:id="rId224" xr:uid="{00000000-0004-0000-0100-0000D2010000}"/>
+    <hyperlink ref="C162" r:id="rId225" xr:uid="{00000000-0004-0000-0100-0000D3010000}"/>
+    <hyperlink ref="C164" r:id="rId226" xr:uid="{00000000-0004-0000-0100-0000D4010000}"/>
+    <hyperlink ref="C165" r:id="rId227" xr:uid="{00000000-0004-0000-0100-0000D5010000}"/>
+    <hyperlink ref="C166" r:id="rId228" xr:uid="{00000000-0004-0000-0100-0000D6010000}"/>
+    <hyperlink ref="C167" r:id="rId229" xr:uid="{00000000-0004-0000-0100-0000D7010000}"/>
+    <hyperlink ref="C168" r:id="rId230" xr:uid="{00000000-0004-0000-0100-0000D8010000}"/>
+    <hyperlink ref="C169" r:id="rId231" xr:uid="{00000000-0004-0000-0100-0000D9010000}"/>
+    <hyperlink ref="C170" r:id="rId232" xr:uid="{00000000-0004-0000-0100-0000DA010000}"/>
+    <hyperlink ref="C171" r:id="rId233" xr:uid="{00000000-0004-0000-0100-0000DB010000}"/>
+    <hyperlink ref="C172" r:id="rId234" xr:uid="{00000000-0004-0000-0100-0000DC010000}"/>
+    <hyperlink ref="C175" r:id="rId235" xr:uid="{00000000-0004-0000-0100-0000DD010000}"/>
+    <hyperlink ref="C176" r:id="rId236" xr:uid="{00000000-0004-0000-0100-0000DE010000}"/>
+    <hyperlink ref="C177" r:id="rId237" xr:uid="{00000000-0004-0000-0100-0000DF010000}"/>
+    <hyperlink ref="C178" r:id="rId238" xr:uid="{00000000-0004-0000-0100-0000E0010000}"/>
+    <hyperlink ref="C181" r:id="rId239" xr:uid="{00000000-0004-0000-0100-0000E1010000}"/>
+    <hyperlink ref="C182" r:id="rId240" xr:uid="{00000000-0004-0000-0100-0000E2010000}"/>
+    <hyperlink ref="C183" r:id="rId241" xr:uid="{00000000-0004-0000-0100-0000E3010000}"/>
+    <hyperlink ref="C184" r:id="rId242" xr:uid="{00000000-0004-0000-0100-0000E4010000}"/>
+    <hyperlink ref="C185" r:id="rId243" xr:uid="{00000000-0004-0000-0100-0000E5010000}"/>
+    <hyperlink ref="C186" r:id="rId244" xr:uid="{00000000-0004-0000-0100-0000E6010000}"/>
+    <hyperlink ref="C187" r:id="rId245" xr:uid="{00000000-0004-0000-0100-0000E7010000}"/>
+    <hyperlink ref="C188" r:id="rId246" xr:uid="{00000000-0004-0000-0100-0000E8010000}"/>
+    <hyperlink ref="C189" r:id="rId247" xr:uid="{00000000-0004-0000-0100-0000E9010000}"/>
+    <hyperlink ref="C190" r:id="rId248" xr:uid="{00000000-0004-0000-0100-0000EA010000}"/>
+    <hyperlink ref="C191" r:id="rId249" xr:uid="{00000000-0004-0000-0100-0000EB010000}"/>
+    <hyperlink ref="C192" r:id="rId250" xr:uid="{00000000-0004-0000-0100-0000EC010000}"/>
+    <hyperlink ref="C196" r:id="rId251" xr:uid="{00000000-0004-0000-0100-0000ED010000}"/>
+    <hyperlink ref="C200" r:id="rId252" xr:uid="{00000000-0004-0000-0100-0000EE010000}"/>
+    <hyperlink ref="C201" r:id="rId253" xr:uid="{00000000-0004-0000-0100-0000EF010000}"/>
+    <hyperlink ref="C202" r:id="rId254" xr:uid="{00000000-0004-0000-0100-0000F0010000}"/>
+    <hyperlink ref="C203" r:id="rId255" xr:uid="{00000000-0004-0000-0100-0000F1010000}"/>
+    <hyperlink ref="C204" r:id="rId256" xr:uid="{00000000-0004-0000-0100-0000F2010000}"/>
+    <hyperlink ref="C205" r:id="rId257" xr:uid="{00000000-0004-0000-0100-0000F3010000}"/>
+    <hyperlink ref="C214" r:id="rId258" xr:uid="{00000000-0004-0000-0100-0000F4010000}"/>
+    <hyperlink ref="C215" r:id="rId259" xr:uid="{00000000-0004-0000-0100-0000F5010000}"/>
+    <hyperlink ref="C216" r:id="rId260" xr:uid="{00000000-0004-0000-0100-0000F6010000}"/>
+    <hyperlink ref="C217" r:id="rId261" xr:uid="{00000000-0004-0000-0100-0000F7010000}"/>
+    <hyperlink ref="C219" r:id="rId262" xr:uid="{00000000-0004-0000-0100-0000F8010000}"/>
+    <hyperlink ref="C220" r:id="rId263" xr:uid="{00000000-0004-0000-0100-0000F9010000}"/>
+    <hyperlink ref="C221" r:id="rId264" xr:uid="{00000000-0004-0000-0100-0000FA010000}"/>
+    <hyperlink ref="C222" r:id="rId265" xr:uid="{00000000-0004-0000-0100-0000FB010000}"/>
+    <hyperlink ref="C223" r:id="rId266" xr:uid="{00000000-0004-0000-0100-0000FC010000}"/>
+    <hyperlink ref="F223" r:id="rId267" xr:uid="{00000000-0004-0000-0100-0000FD010000}"/>
+    <hyperlink ref="C224" r:id="rId268" xr:uid="{00000000-0004-0000-0100-0000FE010000}"/>
+    <hyperlink ref="F224" r:id="rId269" xr:uid="{00000000-0004-0000-0100-0000FF010000}"/>
+    <hyperlink ref="C225" r:id="rId270" xr:uid="{00000000-0004-0000-0100-000000020000}"/>
+    <hyperlink ref="F225" r:id="rId271" xr:uid="{00000000-0004-0000-0100-000001020000}"/>
+    <hyperlink ref="C226" r:id="rId272" xr:uid="{00000000-0004-0000-0100-000002020000}"/>
+    <hyperlink ref="F226" r:id="rId273" xr:uid="{00000000-0004-0000-0100-000003020000}"/>
+    <hyperlink ref="C227" r:id="rId274" xr:uid="{00000000-0004-0000-0100-000004020000}"/>
+    <hyperlink ref="C228" r:id="rId275" xr:uid="{00000000-0004-0000-0100-000005020000}"/>
+    <hyperlink ref="C229" r:id="rId276" xr:uid="{00000000-0004-0000-0100-000006020000}"/>
+    <hyperlink ref="C230" r:id="rId277" xr:uid="{00000000-0004-0000-0100-000007020000}"/>
+    <hyperlink ref="C231" r:id="rId278" xr:uid="{00000000-0004-0000-0100-000008020000}"/>
+    <hyperlink ref="C232" r:id="rId279" xr:uid="{00000000-0004-0000-0100-000009020000}"/>
+    <hyperlink ref="C233" r:id="rId280" xr:uid="{00000000-0004-0000-0100-00000A020000}"/>
+    <hyperlink ref="C234" r:id="rId281" xr:uid="{00000000-0004-0000-0100-00000B020000}"/>
+    <hyperlink ref="C235" r:id="rId282" xr:uid="{00000000-0004-0000-0100-00000C020000}"/>
+    <hyperlink ref="C236" r:id="rId283" xr:uid="{00000000-0004-0000-0100-00000D020000}"/>
+    <hyperlink ref="C237" r:id="rId284" xr:uid="{00000000-0004-0000-0100-00000E020000}"/>
+    <hyperlink ref="C238" r:id="rId285" xr:uid="{00000000-0004-0000-0100-00000F020000}"/>
+    <hyperlink ref="C239" r:id="rId286" xr:uid="{00000000-0004-0000-0100-000010020000}"/>
+    <hyperlink ref="C240" r:id="rId287" xr:uid="{00000000-0004-0000-0100-000011020000}"/>
+    <hyperlink ref="C241" r:id="rId288" xr:uid="{00000000-0004-0000-0100-000012020000}"/>
+    <hyperlink ref="C242" r:id="rId289" xr:uid="{00000000-0004-0000-0100-000013020000}"/>
+    <hyperlink ref="C243" r:id="rId290" xr:uid="{00000000-0004-0000-0100-000014020000}"/>
+    <hyperlink ref="C244" r:id="rId291" xr:uid="{00000000-0004-0000-0100-000015020000}"/>
+    <hyperlink ref="C245" r:id="rId292" xr:uid="{00000000-0004-0000-0100-000016020000}"/>
+    <hyperlink ref="C246" r:id="rId293" xr:uid="{00000000-0004-0000-0100-000017020000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId294"/>
@@ -6335,7 +6335,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Pushing up additional testing files
</commit_message>
<xml_diff>
--- a/testing/test_files/test_genome_annotation.xlsx
+++ b/testing/test_files/test_genome_annotation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1985937\Documents\BI_Sum_2021\EC-Scrape\testing\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFEE7414-EFC1-4D85-9BBA-B15B1DCE58B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{65532160-A043-4581-B43F-CA4782C60C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Genome Annotation" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Pushing up testing files
</commit_message>
<xml_diff>
--- a/testing/test_files/test_genome_annotation.xlsx
+++ b/testing/test_files/test_genome_annotation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1985937\Documents\BI_Sum_2021\EC-Scrape\testing\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54753A0B-795F-483E-B340-569A703ABE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E92A8692-5B22-4E41-8EBB-1FAFCF10905D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Genome Annotation" sheetId="1" r:id="rId1"/>

</xml_diff>